<commit_message>
Updated PBMC template structure, with example dates in correct format
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBBF7FB-745A-7E45-9035-4324F88D8265}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65BB787-327F-9545-ACE9-4324F5867E52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23760" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBMCs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
@@ -164,7 +164,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier account number to pay for shipping if avaialable. Example: 45465732.</t>
+          <t>Courier account number to pay for shipping if available. Example: 45465732.</t>
         </r>
       </text>
     </comment>
@@ -177,7 +177,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of shippment made.</t>
+          <t>Type of shipment made.</t>
         </r>
       </text>
     </comment>
@@ -268,7 +268,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial Participant Identifier. Example: PT123.</t>
         </r>
       </text>
     </comment>
@@ -281,7 +281,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial Participant Identifier. Example: PT123.</t>
+          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
         </r>
       </text>
     </comment>
@@ -294,7 +294,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
+          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
         </r>
       </text>
     </comment>
@@ -307,7 +307,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
+          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
         </r>
       </text>
     </comment>
@@ -320,7 +320,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
+          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
         </r>
       </text>
     </comment>
@@ -333,7 +333,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -346,7 +346,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
         </r>
       </text>
     </comment>
@@ -359,7 +359,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
+          <t>Date of blood collection.</t>
         </r>
       </text>
     </comment>
@@ -372,7 +372,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood collection.</t>
+          <t>Time of blood collection.</t>
         </r>
       </text>
     </comment>
@@ -385,7 +385,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood collection.</t>
+          <t>Date of blood processing.</t>
         </r>
       </text>
     </comment>
@@ -398,7 +398,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood processing.</t>
+          <t>Time of blood processing.</t>
         </r>
       </text>
     </comment>
@@ -411,7 +411,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood processing.</t>
+          <t>Sample location within the shipping container. Example: A1.</t>
         </r>
       </text>
     </comment>
@@ -424,7 +424,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample location within the shipping container. Example: A1.</t>
+          <t>Type of sample sent.</t>
         </r>
       </text>
     </comment>
@@ -437,7 +437,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of sample sent.</t>
+          <t>The format in which the sample was sent.</t>
         </r>
       </text>
     </comment>
@@ -450,7 +450,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The format in which the sample was sent.</t>
+          <t>Quantity of each aliquot shipped.</t>
         </r>
       </text>
     </comment>
@@ -463,7 +463,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Quantity of each sample shipped.</t>
+          <t>Volume of aliquot shipped.</t>
         </r>
       </text>
     </comment>
@@ -476,7 +476,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Volume of sample shipped.</t>
+          <t>The unit of biological material from this aliquot.</t>
         </r>
       </text>
     </comment>
@@ -489,7 +489,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of biological material from this sample.</t>
+          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
         </r>
       </text>
     </comment>
@@ -502,7 +502,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
+          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
         </r>
       </text>
     </comment>
@@ -515,7 +515,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
+          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -528,7 +528,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
         </r>
       </text>
     </comment>
@@ -541,7 +541,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
+          <t>Receiving site indicates how much material was used for assay purposes.</t>
         </r>
       </text>
     </comment>
@@ -554,7 +554,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material was used for assay purposes.</t>
+          <t>Receiving site indicates how much material remains after assay use.</t>
         </r>
       </text>
     </comment>
@@ -567,7 +567,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material remains after assay use.</t>
+          <t>Final status of aliquot after QC and pathology review.</t>
         </r>
       </text>
     </comment>
@@ -580,7 +580,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of sample after QC and pathology review.</t>
+          <t>Status of aliquot if replacement is/was requested.</t>
         </r>
       </text>
     </comment>
@@ -593,20 +593,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Status of sample if replacement is/was requested.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Status of sample used for other assay, exhausted, destroyed, or returned.</t>
+          <t>Status of aliquot used for other assay, exhausted, destroyed, or returned.</t>
         </r>
       </text>
     </comment>
@@ -615,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="75">
   <si>
     <t>#t</t>
   </si>
@@ -818,25 +805,25 @@
     <t>CIMAC-12345</t>
   </si>
   <si>
+    <t>CIMAC-45678</t>
+  </si>
+  <si>
+    <t>CIMAC-54321</t>
+  </si>
+  <si>
+    <t>CIMAC-12354</t>
+  </si>
+  <si>
+    <t>CIMAC-12435</t>
+  </si>
+  <si>
+    <t>CIMAC-14345</t>
+  </si>
+  <si>
     <t>Usable for Assay</t>
   </si>
   <si>
     <t>Replacement Tested</t>
-  </si>
-  <si>
-    <t>CIMAC-45678</t>
-  </si>
-  <si>
-    <t>CIMAC-54321</t>
-  </si>
-  <si>
-    <t>CIMAC-12354</t>
-  </si>
-  <si>
-    <t>CIMAC-12435</t>
-  </si>
-  <si>
-    <t>CIMAC-14345</t>
   </si>
   <si>
     <t>Other</t>
@@ -846,7 +833,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,12 +852,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -939,7 +920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -947,14 +928,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB222"/>
+  <dimension ref="A1:AA222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1305,41 +1287,40 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-    </row>
-    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1373,9 +1354,8 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1409,9 +1389,8 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1445,9 +1424,8 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1481,9 +1459,8 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1517,9 +1494,8 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1553,9 +1529,8 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1589,9 +1564,8 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1625,9 +1599,8 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1661,9 +1634,8 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1697,9 +1669,8 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1733,9 +1704,8 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1769,16 +1739,15 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>41590</v>
       </c>
       <c r="D14" s="1"/>
@@ -1805,9 +1774,8 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-    </row>
-    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1841,9 +1809,8 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1877,9 +1844,8 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-    </row>
-    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1913,9 +1879,8 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-    </row>
-    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1949,9 +1914,8 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-    </row>
-    <row r="19" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1985,659 +1949,636 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB22" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
+        <v>54321</v>
+      </c>
+      <c r="C23">
         <v>12345</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>54321</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>12345</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>54321</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>12345</v>
       </c>
-      <c r="G23">
-        <v>54321</v>
-      </c>
-      <c r="H23">
-        <v>12345</v>
-      </c>
-      <c r="I23" s="4" t="s">
+      <c r="H23" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J23">
+      <c r="I23" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J23" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K23">
         <v>41193</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="6">
         <v>0.42430555555555555</v>
       </c>
-      <c r="L23">
-        <v>41193</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0.42430555555555555</v>
+      <c r="M23" t="s">
+        <v>61</v>
       </c>
       <c r="N23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O23" t="s">
-        <v>62</v>
-      </c>
-      <c r="P23" t="s">
         <v>63</v>
+      </c>
+      <c r="P23">
+        <v>100</v>
       </c>
       <c r="Q23">
         <v>100</v>
       </c>
-      <c r="R23">
+      <c r="R23" t="s">
+        <v>64</v>
+      </c>
+      <c r="S23">
+        <v>10</v>
+      </c>
+      <c r="T23" t="s">
+        <v>65</v>
+      </c>
+      <c r="U23" t="s">
+        <v>66</v>
+      </c>
+      <c r="V23">
+        <v>123</v>
+      </c>
+      <c r="W23">
+        <v>122</v>
+      </c>
+      <c r="X23">
         <v>100</v>
       </c>
-      <c r="S23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T23">
-        <v>10</v>
-      </c>
-      <c r="U23" t="s">
-        <v>65</v>
-      </c>
-      <c r="V23" t="s">
-        <v>66</v>
-      </c>
-      <c r="W23">
-        <v>123</v>
-      </c>
-      <c r="X23">
-        <v>122</v>
-      </c>
-      <c r="Y23">
+      <c r="Y23" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>54321</v>
+      </c>
+      <c r="C24">
+        <v>12345</v>
+      </c>
+      <c r="D24">
+        <v>54321</v>
+      </c>
+      <c r="E24">
+        <v>12345</v>
+      </c>
+      <c r="F24">
+        <v>54321</v>
+      </c>
+      <c r="G24">
+        <v>12345</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K24">
+        <v>41193</v>
+      </c>
+      <c r="L24" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M24" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" t="s">
+        <v>62</v>
+      </c>
+      <c r="O24" t="s">
+        <v>63</v>
+      </c>
+      <c r="P24">
         <v>100</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>12345</v>
-      </c>
-      <c r="C24">
-        <v>54321</v>
-      </c>
-      <c r="D24">
-        <v>12345</v>
-      </c>
-      <c r="E24">
-        <v>54321</v>
-      </c>
-      <c r="F24">
-        <v>12345</v>
-      </c>
-      <c r="G24">
-        <v>54321</v>
-      </c>
-      <c r="H24">
-        <v>12345</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J24">
-        <v>41193</v>
-      </c>
-      <c r="K24" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L24">
-        <v>41193</v>
-      </c>
-      <c r="M24" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N24" t="s">
-        <v>61</v>
-      </c>
-      <c r="O24" t="s">
-        <v>62</v>
-      </c>
-      <c r="P24" t="s">
-        <v>63</v>
       </c>
       <c r="Q24">
         <v>100</v>
       </c>
-      <c r="R24">
+      <c r="R24" t="s">
+        <v>64</v>
+      </c>
+      <c r="S24">
+        <v>10</v>
+      </c>
+      <c r="T24" t="s">
+        <v>65</v>
+      </c>
+      <c r="U24" t="s">
+        <v>67</v>
+      </c>
+      <c r="V24">
+        <v>123</v>
+      </c>
+      <c r="W24">
+        <v>122</v>
+      </c>
+      <c r="X24">
         <v>100</v>
       </c>
-      <c r="S24" t="s">
-        <v>64</v>
-      </c>
-      <c r="T24">
-        <v>10</v>
-      </c>
-      <c r="U24" t="s">
-        <v>65</v>
-      </c>
-      <c r="V24" t="s">
-        <v>69</v>
-      </c>
-      <c r="W24">
-        <v>123</v>
-      </c>
-      <c r="X24">
-        <v>122</v>
-      </c>
-      <c r="Y24">
+      <c r="Y24" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>54321</v>
+      </c>
+      <c r="C25">
+        <v>12345</v>
+      </c>
+      <c r="D25">
+        <v>54321</v>
+      </c>
+      <c r="E25">
+        <v>12345</v>
+      </c>
+      <c r="F25">
+        <v>54321</v>
+      </c>
+      <c r="G25">
+        <v>12345</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K25">
+        <v>41193</v>
+      </c>
+      <c r="L25" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M25" t="s">
+        <v>61</v>
+      </c>
+      <c r="N25" t="s">
+        <v>62</v>
+      </c>
+      <c r="O25" t="s">
+        <v>63</v>
+      </c>
+      <c r="P25">
         <v>100</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>12345</v>
-      </c>
-      <c r="C25">
-        <v>54321</v>
-      </c>
-      <c r="D25">
-        <v>12345</v>
-      </c>
-      <c r="E25">
-        <v>54321</v>
-      </c>
-      <c r="F25">
-        <v>12345</v>
-      </c>
-      <c r="G25">
-        <v>54321</v>
-      </c>
-      <c r="H25">
-        <v>12345</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J25">
-        <v>41193</v>
-      </c>
-      <c r="K25" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L25">
-        <v>41193</v>
-      </c>
-      <c r="M25" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N25" t="s">
-        <v>61</v>
-      </c>
-      <c r="O25" t="s">
-        <v>62</v>
-      </c>
-      <c r="P25" t="s">
-        <v>63</v>
       </c>
       <c r="Q25">
         <v>100</v>
       </c>
-      <c r="R25">
+      <c r="R25" t="s">
+        <v>64</v>
+      </c>
+      <c r="S25">
+        <v>10</v>
+      </c>
+      <c r="T25" t="s">
+        <v>65</v>
+      </c>
+      <c r="U25" t="s">
+        <v>68</v>
+      </c>
+      <c r="V25">
+        <v>123</v>
+      </c>
+      <c r="W25">
+        <v>122</v>
+      </c>
+      <c r="X25">
         <v>100</v>
       </c>
-      <c r="S25" t="s">
-        <v>64</v>
-      </c>
-      <c r="T25">
-        <v>10</v>
-      </c>
-      <c r="U25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V25" t="s">
-        <v>70</v>
-      </c>
-      <c r="W25">
-        <v>123</v>
-      </c>
-      <c r="X25">
-        <v>122</v>
-      </c>
-      <c r="Y25">
+      <c r="Y25" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>54321</v>
+      </c>
+      <c r="C26">
+        <v>12345</v>
+      </c>
+      <c r="D26">
+        <v>54321</v>
+      </c>
+      <c r="E26">
+        <v>12345</v>
+      </c>
+      <c r="F26">
+        <v>54321</v>
+      </c>
+      <c r="G26">
+        <v>12345</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K26">
+        <v>41193</v>
+      </c>
+      <c r="L26" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M26" t="s">
+        <v>61</v>
+      </c>
+      <c r="N26" t="s">
+        <v>62</v>
+      </c>
+      <c r="O26" t="s">
+        <v>63</v>
+      </c>
+      <c r="P26">
         <v>100</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>12345</v>
-      </c>
-      <c r="C26">
-        <v>54321</v>
-      </c>
-      <c r="D26">
-        <v>12345</v>
-      </c>
-      <c r="E26">
-        <v>54321</v>
-      </c>
-      <c r="F26">
-        <v>12345</v>
-      </c>
-      <c r="G26">
-        <v>54321</v>
-      </c>
-      <c r="H26">
-        <v>12345</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26">
-        <v>41193</v>
-      </c>
-      <c r="K26" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L26">
-        <v>41193</v>
-      </c>
-      <c r="M26" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N26" t="s">
-        <v>61</v>
-      </c>
-      <c r="O26" t="s">
-        <v>62</v>
-      </c>
-      <c r="P26" t="s">
-        <v>63</v>
       </c>
       <c r="Q26">
         <v>100</v>
       </c>
-      <c r="R26">
+      <c r="R26" t="s">
+        <v>64</v>
+      </c>
+      <c r="S26">
+        <v>10</v>
+      </c>
+      <c r="T26" t="s">
+        <v>65</v>
+      </c>
+      <c r="U26" t="s">
+        <v>69</v>
+      </c>
+      <c r="V26">
+        <v>123</v>
+      </c>
+      <c r="W26">
+        <v>122</v>
+      </c>
+      <c r="X26">
         <v>100</v>
       </c>
-      <c r="S26" t="s">
-        <v>64</v>
-      </c>
-      <c r="T26">
-        <v>10</v>
-      </c>
-      <c r="U26" t="s">
-        <v>65</v>
-      </c>
-      <c r="V26" t="s">
-        <v>71</v>
-      </c>
-      <c r="W26">
-        <v>123</v>
-      </c>
-      <c r="X26">
-        <v>122</v>
-      </c>
-      <c r="Y26">
+      <c r="Y26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>54321</v>
+      </c>
+      <c r="C27">
+        <v>12345</v>
+      </c>
+      <c r="D27">
+        <v>54321</v>
+      </c>
+      <c r="E27">
+        <v>12345</v>
+      </c>
+      <c r="F27">
+        <v>54321</v>
+      </c>
+      <c r="G27">
+        <v>12345</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J27" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K27">
+        <v>41193</v>
+      </c>
+      <c r="L27" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" t="s">
+        <v>63</v>
+      </c>
+      <c r="P27">
         <v>100</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27">
-        <v>12345</v>
-      </c>
-      <c r="C27">
-        <v>54321</v>
-      </c>
-      <c r="D27">
-        <v>12345</v>
-      </c>
-      <c r="E27">
-        <v>54321</v>
-      </c>
-      <c r="F27">
-        <v>12345</v>
-      </c>
-      <c r="G27">
-        <v>54321</v>
-      </c>
-      <c r="H27">
-        <v>12345</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J27">
-        <v>41193</v>
-      </c>
-      <c r="K27" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L27">
-        <v>41193</v>
-      </c>
-      <c r="M27" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N27" t="s">
-        <v>61</v>
-      </c>
-      <c r="O27" t="s">
-        <v>62</v>
-      </c>
-      <c r="P27" t="s">
-        <v>63</v>
       </c>
       <c r="Q27">
         <v>100</v>
       </c>
-      <c r="R27">
+      <c r="R27" t="s">
+        <v>64</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+      <c r="T27" t="s">
+        <v>65</v>
+      </c>
+      <c r="U27" t="s">
+        <v>70</v>
+      </c>
+      <c r="V27">
+        <v>123</v>
+      </c>
+      <c r="W27">
+        <v>122</v>
+      </c>
+      <c r="X27">
         <v>100</v>
       </c>
-      <c r="S27" t="s">
-        <v>64</v>
-      </c>
-      <c r="T27">
-        <v>10</v>
-      </c>
-      <c r="U27" t="s">
-        <v>65</v>
-      </c>
-      <c r="V27" t="s">
+      <c r="Y27" t="s">
         <v>72</v>
       </c>
-      <c r="W27">
-        <v>123</v>
-      </c>
-      <c r="X27">
-        <v>122</v>
-      </c>
-      <c r="Y27">
+      <c r="Z27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>54321</v>
+      </c>
+      <c r="C28">
+        <v>12345</v>
+      </c>
+      <c r="D28">
+        <v>54321</v>
+      </c>
+      <c r="E28">
+        <v>12345</v>
+      </c>
+      <c r="F28">
+        <v>54321</v>
+      </c>
+      <c r="G28">
+        <v>12345</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K28">
+        <v>41193</v>
+      </c>
+      <c r="L28" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M28" t="s">
+        <v>61</v>
+      </c>
+      <c r="N28" t="s">
+        <v>62</v>
+      </c>
+      <c r="O28" t="s">
+        <v>63</v>
+      </c>
+      <c r="P28">
         <v>100</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>12345</v>
-      </c>
-      <c r="C28">
-        <v>54321</v>
-      </c>
-      <c r="D28">
-        <v>12345</v>
-      </c>
-      <c r="E28">
-        <v>54321</v>
-      </c>
-      <c r="F28">
-        <v>12345</v>
-      </c>
-      <c r="G28">
-        <v>54321</v>
-      </c>
-      <c r="H28">
-        <v>12345</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J28">
-        <v>41193</v>
-      </c>
-      <c r="K28" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L28">
-        <v>41193</v>
-      </c>
-      <c r="M28" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N28" t="s">
-        <v>61</v>
-      </c>
-      <c r="O28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P28" t="s">
-        <v>63</v>
       </c>
       <c r="Q28">
         <v>100</v>
       </c>
-      <c r="R28">
+      <c r="R28" t="s">
+        <v>64</v>
+      </c>
+      <c r="S28">
+        <v>10</v>
+      </c>
+      <c r="T28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U28" t="s">
+        <v>71</v>
+      </c>
+      <c r="V28">
+        <v>123</v>
+      </c>
+      <c r="W28">
+        <v>122</v>
+      </c>
+      <c r="X28">
         <v>100</v>
       </c>
-      <c r="S28" t="s">
-        <v>64</v>
-      </c>
-      <c r="T28">
-        <v>10</v>
-      </c>
-      <c r="U28" t="s">
-        <v>65</v>
-      </c>
-      <c r="V28" t="s">
+      <c r="Y28" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z28" t="s">
         <v>73</v>
       </c>
-      <c r="W28">
-        <v>123</v>
-      </c>
-      <c r="X28">
-        <v>122</v>
-      </c>
-      <c r="Y28">
-        <v>100</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>67</v>
-      </c>
       <c r="AA28" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -3594,46 +3535,49 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:AB1"/>
+    <mergeCell ref="B1:AA1"/>
     <mergeCell ref="B21:U21"/>
-    <mergeCell ref="V21:AB21"/>
+    <mergeCell ref="V21:AA21"/>
   </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{35ED789A-FAD6-644F-AF4C-7A27117F2E28}">
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{F3E6FE57-72BC-A740-8715-EFC67E4B4A18}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{32A2C105-4513-624E-8DCE-3F687C6A3A70}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{CF5C08EF-F396-B04E-BDB1-A22098E080AA}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{A255DB47-7FAB-1743-8154-BDC9C2912DF4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{D6766716-97CD-D448-8D73-8476497F5B74}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{D7FB6114-E406-6045-8227-702A20227734}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{9BC69022-A0AD-C645-82ED-2DA1E8EE9692}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L23:L222 J23:J222" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND(ISNUMBER(J23:J222),LEFT(CELL("format",J23:J222),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K23:K222 I23:I222" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>AND(ISNUMBER(I23:I222),LEFT(CELL("format",I23:I222),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M23:M222 K23:K222" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L23:L222 J23:J222" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N23:N222" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P23:P222" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S23:S222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R23:R222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y23:Y222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA29:AA222" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA28" xr:uid="{984A6193-A151-A644-8F31-8366A7AFC467}">
       <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated docs with desc (#156)
* Updated CyTOF schema

* Re-rendered CyTOF input html #131

* Update test_assays.py

* Clear docs/docs before re-rendering html docs

* Lots of typos and some inconsistent formatting

* Corrected error in mif_input schema #137 

* Update docs with desc

* Ignore .DS_Store files

* Pull excel comments from the 'Description' field (instead of 'Comments')

* Updated PBMC template structure and corresponding example and invalid xlsx. Corrected date format in example values.

* Updated to ignore .DS_Store file

* Update schemas/template/ file sub-directory structure
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBBF7FB-745A-7E45-9035-4324F88D8265}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65BB787-327F-9545-ACE9-4324F5867E52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23760" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBMCs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
@@ -164,7 +164,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier account number to pay for shipping if avaialable. Example: 45465732.</t>
+          <t>Courier account number to pay for shipping if available. Example: 45465732.</t>
         </r>
       </text>
     </comment>
@@ -177,7 +177,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of shippment made.</t>
+          <t>Type of shipment made.</t>
         </r>
       </text>
     </comment>
@@ -268,7 +268,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial Participant Identifier. Example: PT123.</t>
         </r>
       </text>
     </comment>
@@ -281,7 +281,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial Participant Identifier. Example: PT123.</t>
+          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
         </r>
       </text>
     </comment>
@@ -294,7 +294,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
+          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
         </r>
       </text>
     </comment>
@@ -307,7 +307,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the treatment cohort to which the participant belongs. Example: Cohort A.</t>
+          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
         </r>
       </text>
     </comment>
@@ -320,7 +320,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identifies the trial arm to which the participant belongs. Example: Arm A.</t>
+          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
         </r>
       </text>
     </comment>
@@ -333,7 +333,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample identifier assigned by the biorepository site. Example: EA123-45.</t>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -346,7 +346,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
         </r>
       </text>
     </comment>
@@ -359,7 +359,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
+          <t>Date of blood collection.</t>
         </r>
       </text>
     </comment>
@@ -372,7 +372,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood collection.</t>
+          <t>Time of blood collection.</t>
         </r>
       </text>
     </comment>
@@ -385,7 +385,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood collection.</t>
+          <t>Date of blood processing.</t>
         </r>
       </text>
     </comment>
@@ -398,7 +398,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood processing.</t>
+          <t>Time of blood processing.</t>
         </r>
       </text>
     </comment>
@@ -411,7 +411,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood processing.</t>
+          <t>Sample location within the shipping container. Example: A1.</t>
         </r>
       </text>
     </comment>
@@ -424,7 +424,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample location within the shipping container. Example: A1.</t>
+          <t>Type of sample sent.</t>
         </r>
       </text>
     </comment>
@@ -437,7 +437,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of sample sent.</t>
+          <t>The format in which the sample was sent.</t>
         </r>
       </text>
     </comment>
@@ -450,7 +450,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The format in which the sample was sent.</t>
+          <t>Quantity of each aliquot shipped.</t>
         </r>
       </text>
     </comment>
@@ -463,7 +463,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Quantity of each sample shipped.</t>
+          <t>Volume of aliquot shipped.</t>
         </r>
       </text>
     </comment>
@@ -476,7 +476,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Volume of sample shipped.</t>
+          <t>The unit of biological material from this aliquot.</t>
         </r>
       </text>
     </comment>
@@ -489,7 +489,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of biological material from this sample.</t>
+          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
         </r>
       </text>
     </comment>
@@ -502,7 +502,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
+          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
         </r>
       </text>
     </comment>
@@ -515,7 +515,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
+          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
         </r>
       </text>
     </comment>
@@ -528,7 +528,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
         </r>
       </text>
     </comment>
@@ -541,7 +541,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
+          <t>Receiving site indicates how much material was used for assay purposes.</t>
         </r>
       </text>
     </comment>
@@ -554,7 +554,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material was used for assay purposes.</t>
+          <t>Receiving site indicates how much material remains after assay use.</t>
         </r>
       </text>
     </comment>
@@ -567,7 +567,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material remains after assay use.</t>
+          <t>Final status of aliquot after QC and pathology review.</t>
         </r>
       </text>
     </comment>
@@ -580,7 +580,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of sample after QC and pathology review.</t>
+          <t>Status of aliquot if replacement is/was requested.</t>
         </r>
       </text>
     </comment>
@@ -593,20 +593,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Status of sample if replacement is/was requested.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Status of sample used for other assay, exhausted, destroyed, or returned.</t>
+          <t>Status of aliquot used for other assay, exhausted, destroyed, or returned.</t>
         </r>
       </text>
     </comment>
@@ -615,7 +602,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="75">
   <si>
     <t>#t</t>
   </si>
@@ -818,25 +805,25 @@
     <t>CIMAC-12345</t>
   </si>
   <si>
+    <t>CIMAC-45678</t>
+  </si>
+  <si>
+    <t>CIMAC-54321</t>
+  </si>
+  <si>
+    <t>CIMAC-12354</t>
+  </si>
+  <si>
+    <t>CIMAC-12435</t>
+  </si>
+  <si>
+    <t>CIMAC-14345</t>
+  </si>
+  <si>
     <t>Usable for Assay</t>
   </si>
   <si>
     <t>Replacement Tested</t>
-  </si>
-  <si>
-    <t>CIMAC-45678</t>
-  </si>
-  <si>
-    <t>CIMAC-54321</t>
-  </si>
-  <si>
-    <t>CIMAC-12354</t>
-  </si>
-  <si>
-    <t>CIMAC-12435</t>
-  </si>
-  <si>
-    <t>CIMAC-14345</t>
   </si>
   <si>
     <t>Other</t>
@@ -846,7 +833,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -865,12 +852,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -939,7 +920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -947,14 +928,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,10 +1275,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB222"/>
+  <dimension ref="A1:AA222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1305,41 +1287,40 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-    </row>
-    <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+    </row>
+    <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1373,9 +1354,8 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-    </row>
-    <row r="3" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1409,9 +1389,8 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1445,9 +1424,8 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1481,9 +1459,8 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-    </row>
-    <row r="6" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1517,9 +1494,8 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-    </row>
-    <row r="7" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1553,9 +1529,8 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-    </row>
-    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1589,9 +1564,8 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-    </row>
-    <row r="9" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1625,9 +1599,8 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-    </row>
-    <row r="10" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1661,9 +1634,8 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-    </row>
-    <row r="11" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1697,9 +1669,8 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-    </row>
-    <row r="12" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1733,9 +1704,8 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-    </row>
-    <row r="13" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1769,16 +1739,15 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-    </row>
-    <row r="14" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>41590</v>
       </c>
       <c r="D14" s="1"/>
@@ -1805,9 +1774,8 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-    </row>
-    <row r="15" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1841,9 +1809,8 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-    </row>
-    <row r="16" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1877,9 +1844,8 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-    </row>
-    <row r="17" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1913,9 +1879,8 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-    </row>
-    <row r="18" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1949,9 +1914,8 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-    </row>
-    <row r="19" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1985,659 +1949,636 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Z22" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB22" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
+        <v>54321</v>
+      </c>
+      <c r="C23">
         <v>12345</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>54321</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>12345</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>54321</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>12345</v>
       </c>
-      <c r="G23">
-        <v>54321</v>
-      </c>
-      <c r="H23">
-        <v>12345</v>
-      </c>
-      <c r="I23" s="4" t="s">
+      <c r="H23" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="J23">
+      <c r="I23" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J23" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K23">
         <v>41193</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="6">
         <v>0.42430555555555555</v>
       </c>
-      <c r="L23">
-        <v>41193</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0.42430555555555555</v>
+      <c r="M23" t="s">
+        <v>61</v>
       </c>
       <c r="N23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O23" t="s">
-        <v>62</v>
-      </c>
-      <c r="P23" t="s">
         <v>63</v>
+      </c>
+      <c r="P23">
+        <v>100</v>
       </c>
       <c r="Q23">
         <v>100</v>
       </c>
-      <c r="R23">
+      <c r="R23" t="s">
+        <v>64</v>
+      </c>
+      <c r="S23">
+        <v>10</v>
+      </c>
+      <c r="T23" t="s">
+        <v>65</v>
+      </c>
+      <c r="U23" t="s">
+        <v>66</v>
+      </c>
+      <c r="V23">
+        <v>123</v>
+      </c>
+      <c r="W23">
+        <v>122</v>
+      </c>
+      <c r="X23">
         <v>100</v>
       </c>
-      <c r="S23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T23">
-        <v>10</v>
-      </c>
-      <c r="U23" t="s">
-        <v>65</v>
-      </c>
-      <c r="V23" t="s">
-        <v>66</v>
-      </c>
-      <c r="W23">
-        <v>123</v>
-      </c>
-      <c r="X23">
-        <v>122</v>
-      </c>
-      <c r="Y23">
+      <c r="Y23" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>54321</v>
+      </c>
+      <c r="C24">
+        <v>12345</v>
+      </c>
+      <c r="D24">
+        <v>54321</v>
+      </c>
+      <c r="E24">
+        <v>12345</v>
+      </c>
+      <c r="F24">
+        <v>54321</v>
+      </c>
+      <c r="G24">
+        <v>12345</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K24">
+        <v>41193</v>
+      </c>
+      <c r="L24" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M24" t="s">
+        <v>61</v>
+      </c>
+      <c r="N24" t="s">
+        <v>62</v>
+      </c>
+      <c r="O24" t="s">
+        <v>63</v>
+      </c>
+      <c r="P24">
         <v>100</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>12345</v>
-      </c>
-      <c r="C24">
-        <v>54321</v>
-      </c>
-      <c r="D24">
-        <v>12345</v>
-      </c>
-      <c r="E24">
-        <v>54321</v>
-      </c>
-      <c r="F24">
-        <v>12345</v>
-      </c>
-      <c r="G24">
-        <v>54321</v>
-      </c>
-      <c r="H24">
-        <v>12345</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J24">
-        <v>41193</v>
-      </c>
-      <c r="K24" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L24">
-        <v>41193</v>
-      </c>
-      <c r="M24" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N24" t="s">
-        <v>61</v>
-      </c>
-      <c r="O24" t="s">
-        <v>62</v>
-      </c>
-      <c r="P24" t="s">
-        <v>63</v>
       </c>
       <c r="Q24">
         <v>100</v>
       </c>
-      <c r="R24">
+      <c r="R24" t="s">
+        <v>64</v>
+      </c>
+      <c r="S24">
+        <v>10</v>
+      </c>
+      <c r="T24" t="s">
+        <v>65</v>
+      </c>
+      <c r="U24" t="s">
+        <v>67</v>
+      </c>
+      <c r="V24">
+        <v>123</v>
+      </c>
+      <c r="W24">
+        <v>122</v>
+      </c>
+      <c r="X24">
         <v>100</v>
       </c>
-      <c r="S24" t="s">
-        <v>64</v>
-      </c>
-      <c r="T24">
-        <v>10</v>
-      </c>
-      <c r="U24" t="s">
-        <v>65</v>
-      </c>
-      <c r="V24" t="s">
-        <v>69</v>
-      </c>
-      <c r="W24">
-        <v>123</v>
-      </c>
-      <c r="X24">
-        <v>122</v>
-      </c>
-      <c r="Y24">
+      <c r="Y24" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>54321</v>
+      </c>
+      <c r="C25">
+        <v>12345</v>
+      </c>
+      <c r="D25">
+        <v>54321</v>
+      </c>
+      <c r="E25">
+        <v>12345</v>
+      </c>
+      <c r="F25">
+        <v>54321</v>
+      </c>
+      <c r="G25">
+        <v>12345</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J25" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K25">
+        <v>41193</v>
+      </c>
+      <c r="L25" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M25" t="s">
+        <v>61</v>
+      </c>
+      <c r="N25" t="s">
+        <v>62</v>
+      </c>
+      <c r="O25" t="s">
+        <v>63</v>
+      </c>
+      <c r="P25">
         <v>100</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>12345</v>
-      </c>
-      <c r="C25">
-        <v>54321</v>
-      </c>
-      <c r="D25">
-        <v>12345</v>
-      </c>
-      <c r="E25">
-        <v>54321</v>
-      </c>
-      <c r="F25">
-        <v>12345</v>
-      </c>
-      <c r="G25">
-        <v>54321</v>
-      </c>
-      <c r="H25">
-        <v>12345</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J25">
-        <v>41193</v>
-      </c>
-      <c r="K25" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L25">
-        <v>41193</v>
-      </c>
-      <c r="M25" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N25" t="s">
-        <v>61</v>
-      </c>
-      <c r="O25" t="s">
-        <v>62</v>
-      </c>
-      <c r="P25" t="s">
-        <v>63</v>
       </c>
       <c r="Q25">
         <v>100</v>
       </c>
-      <c r="R25">
+      <c r="R25" t="s">
+        <v>64</v>
+      </c>
+      <c r="S25">
+        <v>10</v>
+      </c>
+      <c r="T25" t="s">
+        <v>65</v>
+      </c>
+      <c r="U25" t="s">
+        <v>68</v>
+      </c>
+      <c r="V25">
+        <v>123</v>
+      </c>
+      <c r="W25">
+        <v>122</v>
+      </c>
+      <c r="X25">
         <v>100</v>
       </c>
-      <c r="S25" t="s">
-        <v>64</v>
-      </c>
-      <c r="T25">
-        <v>10</v>
-      </c>
-      <c r="U25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V25" t="s">
-        <v>70</v>
-      </c>
-      <c r="W25">
-        <v>123</v>
-      </c>
-      <c r="X25">
-        <v>122</v>
-      </c>
-      <c r="Y25">
+      <c r="Y25" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>54321</v>
+      </c>
+      <c r="C26">
+        <v>12345</v>
+      </c>
+      <c r="D26">
+        <v>54321</v>
+      </c>
+      <c r="E26">
+        <v>12345</v>
+      </c>
+      <c r="F26">
+        <v>54321</v>
+      </c>
+      <c r="G26">
+        <v>12345</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I26" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J26" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K26">
+        <v>41193</v>
+      </c>
+      <c r="L26" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M26" t="s">
+        <v>61</v>
+      </c>
+      <c r="N26" t="s">
+        <v>62</v>
+      </c>
+      <c r="O26" t="s">
+        <v>63</v>
+      </c>
+      <c r="P26">
         <v>100</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>12345</v>
-      </c>
-      <c r="C26">
-        <v>54321</v>
-      </c>
-      <c r="D26">
-        <v>12345</v>
-      </c>
-      <c r="E26">
-        <v>54321</v>
-      </c>
-      <c r="F26">
-        <v>12345</v>
-      </c>
-      <c r="G26">
-        <v>54321</v>
-      </c>
-      <c r="H26">
-        <v>12345</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26">
-        <v>41193</v>
-      </c>
-      <c r="K26" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L26">
-        <v>41193</v>
-      </c>
-      <c r="M26" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N26" t="s">
-        <v>61</v>
-      </c>
-      <c r="O26" t="s">
-        <v>62</v>
-      </c>
-      <c r="P26" t="s">
-        <v>63</v>
       </c>
       <c r="Q26">
         <v>100</v>
       </c>
-      <c r="R26">
+      <c r="R26" t="s">
+        <v>64</v>
+      </c>
+      <c r="S26">
+        <v>10</v>
+      </c>
+      <c r="T26" t="s">
+        <v>65</v>
+      </c>
+      <c r="U26" t="s">
+        <v>69</v>
+      </c>
+      <c r="V26">
+        <v>123</v>
+      </c>
+      <c r="W26">
+        <v>122</v>
+      </c>
+      <c r="X26">
         <v>100</v>
       </c>
-      <c r="S26" t="s">
-        <v>64</v>
-      </c>
-      <c r="T26">
-        <v>10</v>
-      </c>
-      <c r="U26" t="s">
-        <v>65</v>
-      </c>
-      <c r="V26" t="s">
-        <v>71</v>
-      </c>
-      <c r="W26">
-        <v>123</v>
-      </c>
-      <c r="X26">
-        <v>122</v>
-      </c>
-      <c r="Y26">
+      <c r="Y26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>54321</v>
+      </c>
+      <c r="C27">
+        <v>12345</v>
+      </c>
+      <c r="D27">
+        <v>54321</v>
+      </c>
+      <c r="E27">
+        <v>12345</v>
+      </c>
+      <c r="F27">
+        <v>54321</v>
+      </c>
+      <c r="G27">
+        <v>12345</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J27" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K27">
+        <v>41193</v>
+      </c>
+      <c r="L27" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M27" t="s">
+        <v>61</v>
+      </c>
+      <c r="N27" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" t="s">
+        <v>63</v>
+      </c>
+      <c r="P27">
         <v>100</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27">
-        <v>12345</v>
-      </c>
-      <c r="C27">
-        <v>54321</v>
-      </c>
-      <c r="D27">
-        <v>12345</v>
-      </c>
-      <c r="E27">
-        <v>54321</v>
-      </c>
-      <c r="F27">
-        <v>12345</v>
-      </c>
-      <c r="G27">
-        <v>54321</v>
-      </c>
-      <c r="H27">
-        <v>12345</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J27">
-        <v>41193</v>
-      </c>
-      <c r="K27" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L27">
-        <v>41193</v>
-      </c>
-      <c r="M27" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N27" t="s">
-        <v>61</v>
-      </c>
-      <c r="O27" t="s">
-        <v>62</v>
-      </c>
-      <c r="P27" t="s">
-        <v>63</v>
       </c>
       <c r="Q27">
         <v>100</v>
       </c>
-      <c r="R27">
+      <c r="R27" t="s">
+        <v>64</v>
+      </c>
+      <c r="S27">
+        <v>10</v>
+      </c>
+      <c r="T27" t="s">
+        <v>65</v>
+      </c>
+      <c r="U27" t="s">
+        <v>70</v>
+      </c>
+      <c r="V27">
+        <v>123</v>
+      </c>
+      <c r="W27">
+        <v>122</v>
+      </c>
+      <c r="X27">
         <v>100</v>
       </c>
-      <c r="S27" t="s">
-        <v>64</v>
-      </c>
-      <c r="T27">
-        <v>10</v>
-      </c>
-      <c r="U27" t="s">
-        <v>65</v>
-      </c>
-      <c r="V27" t="s">
+      <c r="Y27" t="s">
         <v>72</v>
       </c>
-      <c r="W27">
-        <v>123</v>
-      </c>
-      <c r="X27">
-        <v>122</v>
-      </c>
-      <c r="Y27">
+      <c r="Z27" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>54321</v>
+      </c>
+      <c r="C28">
+        <v>12345</v>
+      </c>
+      <c r="D28">
+        <v>54321</v>
+      </c>
+      <c r="E28">
+        <v>12345</v>
+      </c>
+      <c r="F28">
+        <v>54321</v>
+      </c>
+      <c r="G28">
+        <v>12345</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" s="7">
+        <v>33234</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K28">
+        <v>41193</v>
+      </c>
+      <c r="L28" s="6">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M28" t="s">
+        <v>61</v>
+      </c>
+      <c r="N28" t="s">
+        <v>62</v>
+      </c>
+      <c r="O28" t="s">
+        <v>63</v>
+      </c>
+      <c r="P28">
         <v>100</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28">
-        <v>12345</v>
-      </c>
-      <c r="C28">
-        <v>54321</v>
-      </c>
-      <c r="D28">
-        <v>12345</v>
-      </c>
-      <c r="E28">
-        <v>54321</v>
-      </c>
-      <c r="F28">
-        <v>12345</v>
-      </c>
-      <c r="G28">
-        <v>54321</v>
-      </c>
-      <c r="H28">
-        <v>12345</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J28">
-        <v>41193</v>
-      </c>
-      <c r="K28" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L28">
-        <v>41193</v>
-      </c>
-      <c r="M28" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N28" t="s">
-        <v>61</v>
-      </c>
-      <c r="O28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P28" t="s">
-        <v>63</v>
       </c>
       <c r="Q28">
         <v>100</v>
       </c>
-      <c r="R28">
+      <c r="R28" t="s">
+        <v>64</v>
+      </c>
+      <c r="S28">
+        <v>10</v>
+      </c>
+      <c r="T28" t="s">
+        <v>65</v>
+      </c>
+      <c r="U28" t="s">
+        <v>71</v>
+      </c>
+      <c r="V28">
+        <v>123</v>
+      </c>
+      <c r="W28">
+        <v>122</v>
+      </c>
+      <c r="X28">
         <v>100</v>
       </c>
-      <c r="S28" t="s">
-        <v>64</v>
-      </c>
-      <c r="T28">
-        <v>10</v>
-      </c>
-      <c r="U28" t="s">
-        <v>65</v>
-      </c>
-      <c r="V28" t="s">
+      <c r="Y28" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z28" t="s">
         <v>73</v>
       </c>
-      <c r="W28">
-        <v>123</v>
-      </c>
-      <c r="X28">
-        <v>122</v>
-      </c>
-      <c r="Y28">
-        <v>100</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>67</v>
-      </c>
       <c r="AA28" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -3594,46 +3535,49 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:AB1"/>
+    <mergeCell ref="B1:AA1"/>
     <mergeCell ref="B21:U21"/>
-    <mergeCell ref="V21:AB21"/>
+    <mergeCell ref="V21:AA21"/>
   </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{35ED789A-FAD6-644F-AF4C-7A27117F2E28}">
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{F3E6FE57-72BC-A740-8715-EFC67E4B4A18}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{32A2C105-4513-624E-8DCE-3F687C6A3A70}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{CF5C08EF-F396-B04E-BDB1-A22098E080AA}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{A255DB47-7FAB-1743-8154-BDC9C2912DF4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{D6766716-97CD-D448-8D73-8476497F5B74}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{D7FB6114-E406-6045-8227-702A20227734}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{9BC69022-A0AD-C645-82ED-2DA1E8EE9692}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L23:L222 J23:J222" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND(ISNUMBER(J23:J222),LEFT(CELL("format",J23:J222),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K23:K222 I23:I222" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>AND(ISNUMBER(I23:I222),LEFT(CELL("format",I23:I222),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M23:M222 K23:K222" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L23:L222 J23:J222" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N23:N222" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P23:P222" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S23:S222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R23:R222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y23:Y222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA29:AA222" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA28" xr:uid="{984A6193-A151-A644-8F31-8366A7AFC467}">
       <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Almost working pbmc - genomic source needs to be added to template schema / xlsx examples
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBBF7FB-745A-7E45-9035-4324F88D8265}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A03F506-1D5A-CF40-A086-7F52ED4B81B0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11300" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PBMCs" sheetId="1" r:id="rId1"/>
+    <sheet name="shipment" sheetId="1" r:id="rId1"/>
+    <sheet name="aliquots" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -56,7 +57,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -69,7 +70,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -259,25 +260,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>CIDC</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{EB3386D3-F9F1-E74C-9496-E6019BF93F5E}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -285,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{1E3CE706-B650-5C47-BC63-E6934412A65B}">
       <text>
         <r>
           <rPr>
@@ -298,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{4560212F-781B-BB4A-9DC3-A564D1CF42B9}">
       <text>
         <r>
           <rPr>
@@ -311,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{34F062A5-F241-EC43-ABFB-9C226DF66B93}">
       <text>
         <r>
           <rPr>
@@ -324,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{5E0CE324-AE1E-714E-9BF4-2F95750CE31F}">
       <text>
         <r>
           <rPr>
@@ -337,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{0C7B6D22-DAB9-C942-8215-1728F79BEC8A}">
       <text>
         <r>
           <rPr>
@@ -350,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{B950FFD6-75B8-DB4E-84DF-98BC0BFEEE5C}">
       <text>
         <r>
           <rPr>
@@ -363,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{F3982C5C-3395-2D44-9037-112C89905579}">
       <text>
         <r>
           <rPr>
@@ -376,7 +374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{2A44BF8F-0B36-0842-B755-5A09070E646E}">
       <text>
         <r>
           <rPr>
@@ -389,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{41579405-D221-B441-82ED-B242C799E2F9}">
       <text>
         <r>
           <rPr>
@@ -402,7 +400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{46F155B8-5896-BD40-AC59-03ADF21C4712}">
       <text>
         <r>
           <rPr>
@@ -415,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{25BC4109-1CBA-484D-80B0-36E4FBBE9992}">
       <text>
         <r>
           <rPr>
@@ -428,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{C0B3A3C3-D841-8647-8D45-7D74D89AD24C}">
       <text>
         <r>
           <rPr>
@@ -441,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{1AF3C62E-3060-2948-88D4-88F8932D3251}">
       <text>
         <r>
           <rPr>
@@ -454,12 +452,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{2F2279BE-F348-F449-A2F0-2D48A273ABE2}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -467,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{EDDB4258-9A2A-B140-B007-103EB331194F}">
       <text>
         <r>
           <rPr>
@@ -480,7 +478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{4B53F284-3F83-284A-9004-068C13397FCD}">
       <text>
         <r>
           <rPr>
@@ -493,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{898C6AD7-5140-DA4E-9921-72B03F339E25}">
       <text>
         <r>
           <rPr>
@@ -506,7 +504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{BE3318F7-8D50-4E46-B8E9-2AE0E3B277FE}">
       <text>
         <r>
           <rPr>
@@ -519,12 +517,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{C1C2EB30-1CA6-1043-8F4E-CEC39D626BAE}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -532,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{ED193828-C491-A046-AD2D-22626D0D5907}">
       <text>
         <r>
           <rPr>
@@ -545,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
+    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{905DB084-99EC-CB4A-8182-7AA99066C099}">
       <text>
         <r>
           <rPr>
@@ -558,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{E356B94D-C485-7542-B1AA-6E29369C8598}">
       <text>
         <r>
           <rPr>
@@ -571,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
+    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{C9484412-C07E-9B48-8EDD-4855AE85FC63}">
       <text>
         <r>
           <rPr>
@@ -584,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
+    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{B7374FD3-6DE1-9F48-904C-4A7799C3F6A2}">
       <text>
         <r>
           <rPr>
@@ -597,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
+    <comment ref="AA3" authorId="0" shapeId="0" xr:uid="{370D81F5-5923-FF43-A618-E6282732AE63}">
       <text>
         <r>
           <rPr>
@@ -615,7 +613,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="82">
   <si>
     <t>#t</t>
   </si>
@@ -815,31 +813,52 @@
     <t>FFPE block #52</t>
   </si>
   <si>
-    <t>CIMAC-12345</t>
-  </si>
-  <si>
     <t>Usable for Assay</t>
   </si>
   <si>
     <t>Replacement Tested</t>
   </si>
   <si>
-    <t>CIMAC-45678</t>
-  </si>
-  <si>
-    <t>CIMAC-54321</t>
-  </si>
-  <si>
-    <t>CIMAC-12354</t>
-  </si>
-  <si>
-    <t>CIMAC-12435</t>
-  </si>
-  <si>
-    <t>CIMAC-14345</t>
-  </si>
-  <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>tPA1</t>
+  </si>
+  <si>
+    <t>PA1</t>
+  </si>
+  <si>
+    <t>PA1SA1</t>
+  </si>
+  <si>
+    <t>tPA2</t>
+  </si>
+  <si>
+    <t>PA2</t>
+  </si>
+  <si>
+    <t>PA2SA2</t>
+  </si>
+  <si>
+    <t>PA1SA1-al1</t>
+  </si>
+  <si>
+    <t>PA1SA1-al2</t>
+  </si>
+  <si>
+    <t>PA1SA1-al3</t>
+  </si>
+  <si>
+    <t>PA2SA2-al4</t>
+  </si>
+  <si>
+    <t>PA2SA2-al5</t>
+  </si>
+  <si>
+    <t>PA2SA2-al6</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
   </si>
 </sst>
 </file>
@@ -901,7 +920,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -935,11 +954,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -952,6 +1008,24 @@
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1293,10 +1367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB222"/>
+  <dimension ref="A1:AB219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1309,35 +1383,35 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
     </row>
     <row r="2" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1346,8 +1420,8 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
-        <v>12345</v>
+      <c r="C2" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1988,639 +2062,34 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="6"/>
-      <c r="V21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6"/>
-      <c r="AB21" s="6"/>
+      <c r="H21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="W22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="X22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB22" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="H22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23">
-        <v>12345</v>
-      </c>
-      <c r="C23">
-        <v>54321</v>
-      </c>
-      <c r="D23">
-        <v>12345</v>
-      </c>
-      <c r="E23">
-        <v>54321</v>
-      </c>
-      <c r="F23">
-        <v>12345</v>
-      </c>
-      <c r="G23">
-        <v>54321</v>
-      </c>
-      <c r="H23">
-        <v>12345</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J23">
-        <v>41193</v>
-      </c>
-      <c r="K23" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L23">
-        <v>41193</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N23" t="s">
-        <v>61</v>
-      </c>
-      <c r="O23" t="s">
-        <v>62</v>
-      </c>
-      <c r="P23" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q23">
-        <v>100</v>
-      </c>
-      <c r="R23">
-        <v>100</v>
-      </c>
-      <c r="S23" t="s">
-        <v>64</v>
-      </c>
-      <c r="T23">
-        <v>10</v>
-      </c>
-      <c r="U23" t="s">
-        <v>65</v>
-      </c>
-      <c r="V23" t="s">
-        <v>66</v>
-      </c>
-      <c r="W23">
-        <v>123</v>
-      </c>
-      <c r="X23">
-        <v>122</v>
-      </c>
-      <c r="Y23">
-        <v>100</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB23" t="s">
-        <v>74</v>
-      </c>
+      <c r="H23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>12345</v>
-      </c>
-      <c r="C24">
-        <v>54321</v>
-      </c>
-      <c r="D24">
-        <v>12345</v>
-      </c>
-      <c r="E24">
-        <v>54321</v>
-      </c>
-      <c r="F24">
-        <v>12345</v>
-      </c>
-      <c r="G24">
-        <v>54321</v>
-      </c>
-      <c r="H24">
-        <v>12345</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J24">
-        <v>41193</v>
-      </c>
-      <c r="K24" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L24">
-        <v>41193</v>
-      </c>
-      <c r="M24" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N24" t="s">
-        <v>61</v>
-      </c>
-      <c r="O24" t="s">
-        <v>62</v>
-      </c>
-      <c r="P24" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q24">
-        <v>100</v>
-      </c>
-      <c r="R24">
-        <v>100</v>
-      </c>
-      <c r="S24" t="s">
-        <v>64</v>
-      </c>
-      <c r="T24">
-        <v>10</v>
-      </c>
-      <c r="U24" t="s">
-        <v>65</v>
-      </c>
-      <c r="V24" t="s">
-        <v>69</v>
-      </c>
-      <c r="W24">
-        <v>123</v>
-      </c>
-      <c r="X24">
-        <v>122</v>
-      </c>
-      <c r="Y24">
-        <v>100</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>74</v>
-      </c>
+      <c r="H24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>12345</v>
-      </c>
-      <c r="C25">
-        <v>54321</v>
-      </c>
-      <c r="D25">
-        <v>12345</v>
-      </c>
-      <c r="E25">
-        <v>54321</v>
-      </c>
-      <c r="F25">
-        <v>12345</v>
-      </c>
-      <c r="G25">
-        <v>54321</v>
-      </c>
-      <c r="H25">
-        <v>12345</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J25">
-        <v>41193</v>
-      </c>
-      <c r="K25" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L25">
-        <v>41193</v>
-      </c>
-      <c r="M25" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N25" t="s">
-        <v>61</v>
-      </c>
-      <c r="O25" t="s">
-        <v>62</v>
-      </c>
-      <c r="P25" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q25">
-        <v>100</v>
-      </c>
-      <c r="R25">
-        <v>100</v>
-      </c>
-      <c r="S25" t="s">
-        <v>64</v>
-      </c>
-      <c r="T25">
-        <v>10</v>
-      </c>
-      <c r="U25" t="s">
-        <v>65</v>
-      </c>
-      <c r="V25" t="s">
-        <v>70</v>
-      </c>
-      <c r="W25">
-        <v>123</v>
-      </c>
-      <c r="X25">
-        <v>122</v>
-      </c>
-      <c r="Y25">
-        <v>100</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>12345</v>
-      </c>
-      <c r="C26">
-        <v>54321</v>
-      </c>
-      <c r="D26">
-        <v>12345</v>
-      </c>
-      <c r="E26">
-        <v>54321</v>
-      </c>
-      <c r="F26">
-        <v>12345</v>
-      </c>
-      <c r="G26">
-        <v>54321</v>
-      </c>
-      <c r="H26">
-        <v>12345</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26">
-        <v>41193</v>
-      </c>
-      <c r="K26" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L26">
-        <v>41193</v>
-      </c>
-      <c r="M26" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N26" t="s">
-        <v>61</v>
-      </c>
-      <c r="O26" t="s">
-        <v>62</v>
-      </c>
-      <c r="P26" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q26">
-        <v>100</v>
-      </c>
-      <c r="R26">
-        <v>100</v>
-      </c>
-      <c r="S26" t="s">
-        <v>64</v>
-      </c>
-      <c r="T26">
-        <v>10</v>
-      </c>
-      <c r="U26" t="s">
-        <v>65</v>
-      </c>
-      <c r="V26" t="s">
-        <v>71</v>
-      </c>
-      <c r="W26">
-        <v>123</v>
-      </c>
-      <c r="X26">
-        <v>122</v>
-      </c>
-      <c r="Y26">
-        <v>100</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27">
-        <v>12345</v>
-      </c>
-      <c r="C27">
-        <v>54321</v>
-      </c>
-      <c r="D27">
-        <v>12345</v>
-      </c>
-      <c r="E27">
-        <v>54321</v>
-      </c>
-      <c r="F27">
-        <v>12345</v>
-      </c>
-      <c r="G27">
-        <v>54321</v>
-      </c>
-      <c r="H27">
-        <v>12345</v>
-      </c>
-      <c r="I27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J27">
-        <v>41193</v>
-      </c>
-      <c r="K27" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L27">
-        <v>41193</v>
-      </c>
-      <c r="M27" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N27" t="s">
-        <v>61</v>
-      </c>
-      <c r="O27" t="s">
-        <v>62</v>
-      </c>
-      <c r="P27" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q27">
-        <v>100</v>
-      </c>
-      <c r="R27">
-        <v>100</v>
-      </c>
-      <c r="S27" t="s">
-        <v>64</v>
-      </c>
-      <c r="T27">
-        <v>10</v>
-      </c>
-      <c r="U27" t="s">
-        <v>65</v>
-      </c>
-      <c r="V27" t="s">
-        <v>72</v>
-      </c>
-      <c r="W27">
-        <v>123</v>
-      </c>
-      <c r="X27">
-        <v>122</v>
-      </c>
-      <c r="Y27">
-        <v>100</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>74</v>
-      </c>
+      <c r="H25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="L25" s="5"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B28">
-        <v>12345</v>
-      </c>
-      <c r="C28">
-        <v>54321</v>
-      </c>
-      <c r="D28">
-        <v>12345</v>
-      </c>
-      <c r="E28">
-        <v>54321</v>
-      </c>
-      <c r="F28">
-        <v>12345</v>
-      </c>
-      <c r="G28">
-        <v>54321</v>
-      </c>
-      <c r="H28">
-        <v>12345</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J28">
-        <v>41193</v>
-      </c>
-      <c r="K28" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="L28">
-        <v>41193</v>
-      </c>
-      <c r="M28" s="5">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="N28" t="s">
-        <v>61</v>
-      </c>
-      <c r="O28" t="s">
-        <v>62</v>
-      </c>
-      <c r="P28" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q28">
-        <v>100</v>
-      </c>
-      <c r="R28">
-        <v>100</v>
-      </c>
-      <c r="S28" t="s">
-        <v>64</v>
-      </c>
-      <c r="T28">
-        <v>10</v>
-      </c>
-      <c r="U28" t="s">
-        <v>65</v>
-      </c>
-      <c r="V28" t="s">
-        <v>73</v>
-      </c>
-      <c r="W28">
-        <v>123</v>
-      </c>
-      <c r="X28">
-        <v>122</v>
-      </c>
-      <c r="Y28">
-        <v>100</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -3577,64 +3046,1688 @@
         <v>24</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A221" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A222" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="B1:AB1"/>
-    <mergeCell ref="B21:U21"/>
-    <mergeCell ref="V21:AB21"/>
   </mergeCells>
-  <dataValidations count="12">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{35ED789A-FAD6-644F-AF4C-7A27117F2E28}">
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{CEF4F657-9B17-3D4E-BEB7-AA512C805C9E}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{32A2C105-4513-624E-8DCE-3F687C6A3A70}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{0508AC2A-D608-2742-B360-C6BD4B978327}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{A255DB47-7FAB-1743-8154-BDC9C2912DF4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{8F51FE5D-A049-2647-AF9A-9F996C2231EE}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{D7FB6114-E406-6045-8227-702A20227734}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{39FEEF23-CBE4-7248-97CE-A76CCDCB9339}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L23:L222 J23:J222" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND(ISNUMBER(J23:J222),LEFT(CELL("format",J23:J222),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L26:L219 J26:J219" xr:uid="{142A586A-7C9A-294A-8DFF-BD228EAC837D}">
+      <formula1>AND(ISNUMBER(J26:J225),LEFT(CELL("format",J26:J225),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M23:M222 K23:K222" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M26:M219 K26:K219 L21:L25 J21:J25" xr:uid="{A4734441-4211-D745-B6D2-9CC614A9576C}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O26:O219 N21:N25" xr:uid="{37B7A701-9B24-054D-8D31-F47801122FEE}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P23:P222" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P26:P219 O21:O25" xr:uid="{70D0F074-FC4B-B942-97DE-D4A2D4E1391D}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S23:S222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S26:S219 R21:R25" xr:uid="{5F1B1B1D-ACF3-144C-BDFE-5A40FF86BF7F}">
       <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z26:Z219 Y21:Y25" xr:uid="{EFDA8D82-62D3-914F-95CC-94B96EE5BD9F}">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA26:AA219 Z21:Z25" xr:uid="{62F7AA30-EDCF-A344-959F-99FE519F4AF1}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB23:AB222" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB26:AB219 AA21:AA25" xr:uid="{CCA786E5-3820-964D-9D71-23F86EFA5623}">
       <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K21:K25 I21:I25" xr:uid="{1C904381-45E6-E043-A765-F11CB6C61550}">
+      <formula1>AND(ISNUMBER(J21:J220),LEFT(CELL("format",J21:J220),1)="D")</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B9C197-8600-D943-8391-ECAEAF59EB82}">
+  <dimension ref="A2:AB203"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="11"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4">
+        <v>54321</v>
+      </c>
+      <c r="E4">
+        <v>12345</v>
+      </c>
+      <c r="F4">
+        <v>54321</v>
+      </c>
+      <c r="G4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>41193</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K4">
+        <v>41193</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+      <c r="R4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S4">
+        <v>10</v>
+      </c>
+      <c r="T4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" t="s">
+        <v>75</v>
+      </c>
+      <c r="V4">
+        <v>123</v>
+      </c>
+      <c r="W4">
+        <v>122</v>
+      </c>
+      <c r="X4">
+        <v>100</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>54321</v>
+      </c>
+      <c r="E5">
+        <v>12345</v>
+      </c>
+      <c r="F5">
+        <v>54321</v>
+      </c>
+      <c r="G5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>41193</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K5">
+        <v>41193</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+      <c r="R5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5">
+        <v>10</v>
+      </c>
+      <c r="T5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" t="s">
+        <v>76</v>
+      </c>
+      <c r="V5">
+        <v>123</v>
+      </c>
+      <c r="W5">
+        <v>122</v>
+      </c>
+      <c r="X5">
+        <v>100</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6">
+        <v>54321</v>
+      </c>
+      <c r="E6">
+        <v>12345</v>
+      </c>
+      <c r="F6">
+        <v>54321</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6">
+        <v>41193</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K6">
+        <v>41193</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6">
+        <v>100</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+      <c r="R6" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6">
+        <v>10</v>
+      </c>
+      <c r="T6" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" t="s">
+        <v>77</v>
+      </c>
+      <c r="V6">
+        <v>123</v>
+      </c>
+      <c r="W6">
+        <v>122</v>
+      </c>
+      <c r="X6">
+        <v>100</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7">
+        <v>54321</v>
+      </c>
+      <c r="E7">
+        <v>12345</v>
+      </c>
+      <c r="F7">
+        <v>54321</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7">
+        <v>41193</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K7">
+        <v>41193</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="R7" t="s">
+        <v>64</v>
+      </c>
+      <c r="S7">
+        <v>10</v>
+      </c>
+      <c r="T7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" t="s">
+        <v>78</v>
+      </c>
+      <c r="V7">
+        <v>123</v>
+      </c>
+      <c r="W7">
+        <v>122</v>
+      </c>
+      <c r="X7">
+        <v>100</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8">
+        <v>54321</v>
+      </c>
+      <c r="E8">
+        <v>12345</v>
+      </c>
+      <c r="F8">
+        <v>54321</v>
+      </c>
+      <c r="G8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8">
+        <v>41193</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K8">
+        <v>41193</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8" t="s">
+        <v>64</v>
+      </c>
+      <c r="S8">
+        <v>10</v>
+      </c>
+      <c r="T8" t="s">
+        <v>65</v>
+      </c>
+      <c r="U8" t="s">
+        <v>79</v>
+      </c>
+      <c r="V8">
+        <v>123</v>
+      </c>
+      <c r="W8">
+        <v>122</v>
+      </c>
+      <c r="X8">
+        <v>100</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9">
+        <v>54321</v>
+      </c>
+      <c r="E9">
+        <v>12345</v>
+      </c>
+      <c r="F9">
+        <v>54321</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9">
+        <v>41193</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K9">
+        <v>41193</v>
+      </c>
+      <c r="L9" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9">
+        <v>100</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+      <c r="R9" t="s">
+        <v>64</v>
+      </c>
+      <c r="S9">
+        <v>10</v>
+      </c>
+      <c r="T9" t="s">
+        <v>65</v>
+      </c>
+      <c r="U9" t="s">
+        <v>80</v>
+      </c>
+      <c r="V9">
+        <v>123</v>
+      </c>
+      <c r="W9">
+        <v>122</v>
+      </c>
+      <c r="X9">
+        <v>100</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:U2"/>
+    <mergeCell ref="V2:AB2"/>
+  </mergeCells>
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB10:AB203 AA4:AA9" xr:uid="{973DDE31-29F8-3946-9F57-C350CEE2F8E5}">
+      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA10:AA203 Z4:Z9" xr:uid="{53B89728-DB3D-7146-83FC-81A0423FBB10}">
+      <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z10:Z203 Y4:Y9" xr:uid="{8A57EB6E-B549-7F41-95CA-058366A210CA}">
+      <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S10:S203 R4:R9" xr:uid="{FDA9BFC4-3089-D140-8BAB-994C4312A18E}">
+      <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P10:P203 O4:O9" xr:uid="{B8785C88-AD14-6A42-AC09-8E7503E8BCF8}">
+      <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O10:O203 N4:N9" xr:uid="{4BF5B0E7-5C7E-524F-8090-D912731210DB}">
+      <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M10:M203 J4:J9 K10:K203 L4:L9" xr:uid="{A9095E68-E922-DE4F-8BE7-39F9D59C1209}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555555</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K4:K9 I4:I9" xr:uid="{942F830A-8796-0B47-89A8-B18B970FCC09}">
+      <formula1>AND(ISNUMBER(J4:J203),LEFT(CELL("format",J4:J203),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L10:L203 J10:J203" xr:uid="{74A534CB-251F-744A-AD1F-2EBE6269F401}">
+      <formula1>AND(ISNUMBER(J10:J209),LEFT(CELL("format",J10:J209),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
plasma_template updated for new prism
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C9882-C3A9-CF40-AFE0-053227DA92F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE9C329-BC3B-1440-B2B1-05E4D95ADD02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="460" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shipment" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -600,7 +600,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -772,15 +772,6 @@
     <t>MATERIAL REMAINING</t>
   </si>
   <si>
-    <t>SAMPLE QUALITY STATUS</t>
-  </si>
-  <si>
-    <t>SAMPLE REPLACEMENT</t>
-  </si>
-  <si>
-    <t>SAMPLE STATUS</t>
-  </si>
-  <si>
     <t>R123</t>
   </si>
   <si>
@@ -890,6 +881,15 @@
   </si>
   <si>
     <t>PA2SA1-al5</t>
+  </si>
+  <si>
+    <t>ALIQUOT QUALITY STATUS</t>
+  </si>
+  <si>
+    <t>ALIQUOT REPLACEMENT</t>
+  </si>
+  <si>
+    <t>ALIQUOT STATUS</t>
   </si>
 </sst>
 </file>
@@ -1452,7 +1452,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1524,7 +1524,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1560,7 +1560,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1596,7 +1596,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1740,7 +1740,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1776,7 +1776,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1812,7 +1812,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1848,7 +1848,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2028,7 +2028,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2064,7 +2064,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3132,8 +3132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B9C197-8600-D943-8391-ECAEAF59EB82}">
   <dimension ref="A2:AB203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3201,7 +3201,7 @@
         <v>31</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>32</v>
@@ -3252,13 +3252,13 @@
         <v>47</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -3266,10 +3266,10 @@
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4">
         <v>54321</v>
@@ -3281,13 +3281,13 @@
         <v>54321</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J4">
         <v>41193</v>
@@ -3302,13 +3302,13 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="N4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q4">
         <v>100</v>
@@ -3317,16 +3317,16 @@
         <v>100</v>
       </c>
       <c r="S4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="T4">
         <v>10</v>
       </c>
       <c r="U4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="V4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="W4">
         <v>123</v>
@@ -3338,13 +3338,13 @@
         <v>100</v>
       </c>
       <c r="Z4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AA4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AB4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
@@ -3352,10 +3352,10 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D5">
         <v>54321</v>
@@ -3367,13 +3367,13 @@
         <v>54321</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J5">
         <v>41193</v>
@@ -3388,13 +3388,13 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="N5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q5">
         <v>100</v>
@@ -3403,16 +3403,16 @@
         <v>100</v>
       </c>
       <c r="S5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="T5">
         <v>10</v>
       </c>
       <c r="U5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="V5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="W5">
         <v>123</v>
@@ -3424,13 +3424,13 @@
         <v>100</v>
       </c>
       <c r="Z5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AA5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AB5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -3438,10 +3438,10 @@
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D6">
         <v>54321</v>
@@ -3453,13 +3453,13 @@
         <v>54321</v>
       </c>
       <c r="G6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J6">
         <v>41193</v>
@@ -3474,13 +3474,13 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="N6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q6">
         <v>100</v>
@@ -3489,16 +3489,16 @@
         <v>100</v>
       </c>
       <c r="S6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="T6">
         <v>10</v>
       </c>
       <c r="U6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="V6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="W6">
         <v>123</v>
@@ -3510,13 +3510,13 @@
         <v>100</v>
       </c>
       <c r="Z6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AA6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AB6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -3524,10 +3524,10 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D7">
         <v>54321</v>
@@ -3539,13 +3539,13 @@
         <v>54321</v>
       </c>
       <c r="G7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J7">
         <v>41193</v>
@@ -3560,13 +3560,13 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="N7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q7">
         <v>100</v>
@@ -3575,16 +3575,16 @@
         <v>100</v>
       </c>
       <c r="S7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="T7">
         <v>10</v>
       </c>
       <c r="U7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="V7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="W7">
         <v>123</v>
@@ -3596,13 +3596,13 @@
         <v>100</v>
       </c>
       <c r="Z7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AA7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AB7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
@@ -3610,10 +3610,10 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D8">
         <v>54321</v>
@@ -3625,13 +3625,13 @@
         <v>54321</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J8">
         <v>41193</v>
@@ -3646,13 +3646,13 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="N8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q8">
         <v>100</v>
@@ -3661,16 +3661,16 @@
         <v>100</v>
       </c>
       <c r="S8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="T8">
         <v>10</v>
       </c>
       <c r="U8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="V8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="W8">
         <v>123</v>
@@ -3682,13 +3682,13 @@
         <v>100</v>
       </c>
       <c r="Z8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AA8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AB8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -3696,10 +3696,10 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D9">
         <v>54321</v>
@@ -3711,13 +3711,13 @@
         <v>54321</v>
       </c>
       <c r="G9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J9">
         <v>41193</v>
@@ -3732,13 +3732,13 @@
         <v>0.42430555555555555</v>
       </c>
       <c r="N9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="O9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="P9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q9">
         <v>100</v>
@@ -3747,16 +3747,16 @@
         <v>100</v>
       </c>
       <c r="S9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="T9">
         <v>10</v>
       </c>
       <c r="U9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="V9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="W9">
         <v>123</v>
@@ -3768,13 +3768,13 @@
         <v>100</v>
       </c>
       <c r="Z9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="AA9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="AB9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Make sure all fields in a template schema exist in a template
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE9C329-BC3B-1440-B2B1-05E4D95ADD02}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A909C8E-46EF-6F4F-B952-BFC800EBBA32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="620" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shipment" sheetId="1" r:id="rId1"/>
@@ -853,9 +853,6 @@
     <t>PA2SA2-al6</t>
   </si>
   <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
     <t>GENOMIC SOURCE</t>
   </si>
   <si>
@@ -890,6 +887,9 @@
   </si>
   <si>
     <t>ALIQUOT STATUS</t>
+  </si>
+  <si>
+    <t>staging_0</t>
   </si>
 </sst>
 </file>
@@ -1400,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB219"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1452,7 +1452,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3132,8 +3132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B9C197-8600-D943-8391-ECAEAF59EB82}">
   <dimension ref="A2:AB203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3201,7 +3201,7 @@
         <v>31</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>32</v>
@@ -3252,13 +3252,13 @@
         <v>47</v>
       </c>
       <c r="Z3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -3287,7 +3287,7 @@
         <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J4">
         <v>41193</v>
@@ -3373,7 +3373,7 @@
         <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J5">
         <v>41193</v>
@@ -3453,13 +3453,13 @@
         <v>54321</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J6">
         <v>41193</v>
@@ -3498,7 +3498,7 @@
         <v>62</v>
       </c>
       <c r="V6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="W6">
         <v>123</v>
@@ -3539,13 +3539,13 @@
         <v>54321</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J7">
         <v>41193</v>
@@ -3584,7 +3584,7 @@
         <v>62</v>
       </c>
       <c r="V7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W7">
         <v>123</v>
@@ -3625,13 +3625,13 @@
         <v>54321</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J8">
         <v>41193</v>
@@ -3670,7 +3670,7 @@
         <v>62</v>
       </c>
       <c r="V8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="W8">
         <v>123</v>
@@ -3714,10 +3714,10 @@
         <v>71</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J9">
         <v>41193</v>

</xml_diff>

<commit_message>
pbmc template (and example) changes from NCI 9/24 feedback
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{502317B3-046A-B241-BBF8-DB67092C913C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9562E226-8607-304F-89F0-7520C04DCA1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23680" windowHeight="12040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25660" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -708,7 +708,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Site or biobank provides the final number of PBMCs per vial that were frozen.</t>
+          <t>Receiving site determines the percent recovered cells that are viable after thawing.</t>
         </r>
       </text>
     </comment>
@@ -721,7 +721,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site determines number fo PBMCs per vial recovered upon receipt.</t>
+          <t>Receiving site determines number for PBMCs per vial recovered upon receipt.</t>
         </r>
       </text>
     </comment>
@@ -734,7 +734,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material was used for assay purposes.</t>
+          <t>Receiving site indicates if a resting period was used after PBMC recovery.</t>
         </r>
       </text>
     </comment>
@@ -747,7 +747,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material remains after assay use.</t>
+          <t>Receiving site indicates how much material was used for assay purposes.</t>
         </r>
       </text>
     </comment>
@@ -760,7 +760,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indication if sample replacement is/was requested.</t>
+          <t>Receiving site indicates how much material remains after assay use.</t>
         </r>
       </text>
     </comment>
@@ -773,11 +773,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Indication if sample replacement is/was requested.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Indication if sample was sent to another location or returned back to biorepository.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -795,7 +808,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="122">
   <si>
     <t>#t</t>
   </si>
@@ -971,10 +984,13 @@
     <t>SAMPLE VOLUME UNITS</t>
   </si>
   <si>
-    <t>PBMC FROZEN</t>
-  </si>
-  <si>
-    <t>PBMC RECOVERED</t>
+    <t>PBMC VIABILITY</t>
+  </si>
+  <si>
+    <t>PBMC RECOVERY</t>
+  </si>
+  <si>
+    <t>PBMC RESTING PERIOD USED</t>
   </si>
   <si>
     <t>MATERIAL USED</t>
@@ -1164,7 +1180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1185,13 +1201,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1220,7 +1229,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1254,15 +1263,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1272,13 +1300,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="21" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1619,8 +1651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1633,293 +1665,293 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="C2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>99</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>99</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>123</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5">
-        <v>41590</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="8">
+        <v>36892</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5">
-        <v>41590</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="8">
+        <v>36892</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>8</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>8</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>8</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2931,19 +2963,19 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{684EBF91-2934-A842-8094-2A805A1B3BC6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{FC9D57D1-BBC4-B643-A513-5833F7B8478F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{9FC9EDAF-BFF8-4746-A281-0CDCCFFF871E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14:C15" xr:uid="{7A0AA3F8-77D1-8C44-9D3D-99B4A47830A7}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14:C15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0A8C0828-0B9F-EF40-B7CD-DFB4695992D9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Specimen shipment received in good condition,Specimen shipment received in poor condition,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2957,7 +2989,7 @@
   <dimension ref="A1:K202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD8"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2966,55 +2998,56 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3022,210 +3055,210 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="C3" t="s">
         <v>79</v>
       </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
       <c r="E3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
       <c r="I3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" t="s">
         <v>87</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" t="s">
-        <v>85</v>
-      </c>
-      <c r="K4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="7" t="s">
+      <c r="B5" t="s">
         <v>89</v>
       </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
       <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="H5" t="s">
+        <v>84</v>
+      </c>
       <c r="I5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>78</v>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H6" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="H6" t="s">
+        <v>84</v>
+      </c>
       <c r="I6" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I7" t="s">
+        <v>92</v>
+      </c>
+      <c r="J7" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" t="s">
         <v>94</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I7" t="s">
-        <v>91</v>
-      </c>
-      <c r="J7" t="s">
-        <v>92</v>
-      </c>
-      <c r="K7" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>89</v>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="6" t="s">
         <v>80</v>
       </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H8" s="6" t="s">
         <v>83</v>
       </c>
+      <c r="H8" t="s">
+        <v>84</v>
+      </c>
       <c r="I8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -4199,15 +4232,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D202" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D202" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"ACCESSORY SINUS, NOS,ADRENAL GLANDS,ANAL CANAL &amp; ANUS,APPENDIX,BASE OF TONGUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E202 E3:E4" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E202" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"C00,C00.0,C00.1,C00.2,C00.3,C00.4,C00.5,C00.6,C00.8,C00.9,C01,C01.9"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F202" xr:uid="{00000000-0002-0000-0100-000002000000}">
@@ -4216,7 +4250,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G202" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"8000/3,8001/3,8002/3,8003/3,8004/3,8005/3,8010/2,8010/3,8011/3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H202" xr:uid="{00000000-0002-0000-0100-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H202" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"Neoplasm, malignant,Tumor cells, malignant,Malignant tumor, small cell type,Malignant tumor, giant cell type,Malignant tumor, spindle cell type,Malignant tumor, clear cell type"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000005000000}">
@@ -4236,10 +4270,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AB202"/>
+  <dimension ref="A1:AC202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD8"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4248,179 +4282,183 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC2" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>96</v>
+      <c r="B3" t="s">
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>77</v>
+        <v>101</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>102</v>
-      </c>
-      <c r="J3" s="8">
-        <v>37174</v>
-      </c>
-      <c r="K3" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L3" s="8">
-        <v>37174</v>
-      </c>
-      <c r="M3" s="9">
-        <v>0.33333333333333331</v>
+        <v>103</v>
+      </c>
+      <c r="J3" s="6">
+        <v>36892</v>
+      </c>
+      <c r="K3" s="7">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="L3" s="6">
+        <v>36892</v>
+      </c>
+      <c r="M3" s="7">
+        <v>4.9305555555555554E-2</v>
       </c>
       <c r="N3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O3">
         <v>123</v>
       </c>
       <c r="P3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -4429,7 +4467,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V3">
         <v>1</v>
@@ -4441,10 +4479,10 @@
         <v>1</v>
       </c>
       <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
         <v>0</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>108</v>
       </c>
       <c r="AA3" t="s">
         <v>109</v>
@@ -4452,61 +4490,64 @@
       <c r="AB3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>111</v>
+      <c r="B4" t="s">
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>87</v>
+        <v>101</v>
+      </c>
+      <c r="G4" t="s">
+        <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
-      </c>
-      <c r="J4" s="8">
-        <v>37174</v>
-      </c>
-      <c r="K4" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L4" s="8">
-        <v>37174</v>
-      </c>
-      <c r="M4" s="9">
-        <v>0.33333333333333331</v>
+        <v>103</v>
+      </c>
+      <c r="J4" s="6">
+        <v>36892</v>
+      </c>
+      <c r="K4" s="7">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="L4" s="6">
+        <v>36892</v>
+      </c>
+      <c r="M4" s="7">
+        <v>4.9305555555555554E-2</v>
       </c>
       <c r="N4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O4">
         <v>123</v>
       </c>
       <c r="P4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -4515,7 +4556,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V4">
         <v>1</v>
@@ -4527,10 +4568,10 @@
         <v>1</v>
       </c>
       <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
         <v>0</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>108</v>
       </c>
       <c r="AA4" t="s">
         <v>109</v>
@@ -4538,61 +4579,64 @@
       <c r="AB4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>113</v>
+      <c r="B5" t="s">
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>88</v>
+        <v>101</v>
+      </c>
+      <c r="G5" t="s">
+        <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J5" s="8">
-        <v>37174</v>
-      </c>
-      <c r="K5" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L5" s="8">
-        <v>37174</v>
-      </c>
-      <c r="M5" s="9">
-        <v>0.33333333333333331</v>
+        <v>103</v>
+      </c>
+      <c r="J5" s="6">
+        <v>36892</v>
+      </c>
+      <c r="K5" s="7">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="L5" s="6">
+        <v>36892</v>
+      </c>
+      <c r="M5" s="7">
+        <v>4.9305555555555554E-2</v>
       </c>
       <c r="N5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O5">
         <v>123</v>
       </c>
       <c r="P5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -4601,7 +4645,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V5">
         <v>1</v>
@@ -4613,10 +4657,10 @@
         <v>1</v>
       </c>
       <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
         <v>0</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>108</v>
       </c>
       <c r="AA5" t="s">
         <v>109</v>
@@ -4624,61 +4668,64 @@
       <c r="AB5" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>115</v>
+      <c r="B6" t="s">
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>90</v>
+        <v>101</v>
+      </c>
+      <c r="G6" t="s">
+        <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>102</v>
-      </c>
-      <c r="J6" s="8">
-        <v>37174</v>
-      </c>
-      <c r="K6" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L6" s="8">
-        <v>37174</v>
-      </c>
-      <c r="M6" s="9">
-        <v>0.33333333333333331</v>
+        <v>103</v>
+      </c>
+      <c r="J6" s="6">
+        <v>36892</v>
+      </c>
+      <c r="K6" s="7">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="L6" s="6">
+        <v>36892</v>
+      </c>
+      <c r="M6" s="7">
+        <v>4.9305555555555554E-2</v>
       </c>
       <c r="N6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O6">
         <v>123</v>
       </c>
       <c r="P6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -4687,7 +4734,7 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V6">
         <v>1</v>
@@ -4699,10 +4746,10 @@
         <v>1</v>
       </c>
       <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
         <v>0</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>108</v>
       </c>
       <c r="AA6" t="s">
         <v>109</v>
@@ -4710,61 +4757,64 @@
       <c r="AB6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>117</v>
+      <c r="B7" t="s">
+        <v>118</v>
       </c>
       <c r="C7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>94</v>
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
+        <v>95</v>
       </c>
       <c r="H7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
-      </c>
-      <c r="J7" s="8">
-        <v>37174</v>
-      </c>
-      <c r="K7" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L7" s="8">
-        <v>37174</v>
-      </c>
-      <c r="M7" s="9">
-        <v>0.33333333333333331</v>
+        <v>103</v>
+      </c>
+      <c r="J7" s="6">
+        <v>36892</v>
+      </c>
+      <c r="K7" s="7">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="L7" s="6">
+        <v>36892</v>
+      </c>
+      <c r="M7" s="7">
+        <v>4.9305555555555554E-2</v>
       </c>
       <c r="N7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O7">
         <v>123</v>
       </c>
       <c r="P7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -4773,7 +4823,7 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V7">
         <v>1</v>
@@ -4785,10 +4835,10 @@
         <v>1</v>
       </c>
       <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
         <v>0</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>108</v>
       </c>
       <c r="AA7" t="s">
         <v>109</v>
@@ -4796,61 +4846,64 @@
       <c r="AB7" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>119</v>
+      <c r="B8" t="s">
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>95</v>
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>96</v>
       </c>
       <c r="H8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>102</v>
-      </c>
-      <c r="J8" s="8">
-        <v>37174</v>
-      </c>
-      <c r="K8" s="9">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="L8" s="8">
-        <v>37174</v>
-      </c>
-      <c r="M8" s="9">
-        <v>0.33333333333333331</v>
+        <v>103</v>
+      </c>
+      <c r="J8" s="6">
+        <v>36892</v>
+      </c>
+      <c r="K8" s="7">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="L8" s="6">
+        <v>36892</v>
+      </c>
+      <c r="M8" s="7">
+        <v>4.9305555555555554E-2</v>
       </c>
       <c r="N8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="O8">
         <v>123</v>
       </c>
       <c r="P8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Q8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="R8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -4859,7 +4912,7 @@
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V8">
         <v>1</v>
@@ -4871,10 +4924,10 @@
         <v>1</v>
       </c>
       <c r="Y8">
+        <v>1</v>
+      </c>
+      <c r="Z8">
         <v>0</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>108</v>
       </c>
       <c r="AA8" t="s">
         <v>109</v>
@@ -4882,43 +4935,46 @@
       <c r="AB8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AC8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5855,17 +5911,17 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:V1"/>
-    <mergeCell ref="W1:AB1"/>
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="V1:AC1"/>
   </mergeCells>
-  <dataValidations count="11">
+  <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L3:L202 J3:J202" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="J3:J202 L3:L202" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>AND(ISNUMBER(J3:J202),LEFT(CELL("format",J3:J202),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M3:M202 K3:K202" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="K3:K202 M3:M202" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
@@ -5884,14 +5940,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U202" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"Microliter,Milliliter,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3:Z202" xr:uid="{00000000-0002-0000-0200-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA9:AA202 AB3:AB8" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA202" xr:uid="{00000000-0002-0000-0200-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB9:AB202 AC3:AC8" xr:uid="{00000000-0002-0000-0200-00000B000000}">
       <formula1>"Sample Returned,Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y8" xr:uid="{ADE444BB-42AD-C848-B6D5-1F8F18406671}">
-      <formula1>"Microliters,Milliliters,Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
pbmc resting period - enum
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9562E226-8607-304F-89F0-7520C04DCA1D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBCE047-0578-7841-A110-56451E8CAB08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25660" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25660" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -808,7 +808,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="125">
   <si>
     <t>#t</t>
   </si>
@@ -1174,6 +1174,15 @@
   </si>
   <si>
     <t>TRIALGROUP 6</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -1297,6 +1306,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1305,11 +1319,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1651,7 +1660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1665,13 +1674,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1848,7 +1857,7 @@
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="5">
         <v>36892</v>
       </c>
       <c r="D14" s="1"/>
@@ -1862,7 +1871,7 @@
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="5">
         <v>36892</v>
       </c>
       <c r="D15" s="1"/>
@@ -2999,22 +3008,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -4272,8 +4281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AC202"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4283,38 +4292,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -4433,16 +4442,16 @@
       <c r="I3" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="3">
         <v>36892</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="3">
         <v>36892</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
       <c r="N3" t="s">
@@ -4475,8 +4484,8 @@
       <c r="W3">
         <v>1</v>
       </c>
-      <c r="X3">
-        <v>1</v>
+      <c r="X3" t="s">
+        <v>122</v>
       </c>
       <c r="Y3">
         <v>1</v>
@@ -4522,16 +4531,16 @@
       <c r="I4" t="s">
         <v>103</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="3">
         <v>36892</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="3">
         <v>36892</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
       <c r="N4" t="s">
@@ -4564,8 +4573,8 @@
       <c r="W4">
         <v>1</v>
       </c>
-      <c r="X4">
-        <v>1</v>
+      <c r="X4" t="s">
+        <v>123</v>
       </c>
       <c r="Y4">
         <v>1</v>
@@ -4611,16 +4620,16 @@
       <c r="I5" t="s">
         <v>103</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="3">
         <v>36892</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="3">
         <v>36892</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
       <c r="N5" t="s">
@@ -4653,8 +4662,8 @@
       <c r="W5">
         <v>1</v>
       </c>
-      <c r="X5">
-        <v>1</v>
+      <c r="X5" t="s">
+        <v>108</v>
       </c>
       <c r="Y5">
         <v>1</v>
@@ -4700,16 +4709,16 @@
       <c r="I6" t="s">
         <v>103</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="3">
         <v>36892</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="3">
         <v>36892</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
       <c r="N6" t="s">
@@ -4742,8 +4751,8 @@
       <c r="W6">
         <v>1</v>
       </c>
-      <c r="X6">
-        <v>1</v>
+      <c r="X6" t="s">
+        <v>124</v>
       </c>
       <c r="Y6">
         <v>1</v>
@@ -4789,16 +4798,16 @@
       <c r="I7" t="s">
         <v>103</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="3">
         <v>36892</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="3">
         <v>36892</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
       <c r="N7" t="s">
@@ -4831,8 +4840,8 @@
       <c r="W7">
         <v>1</v>
       </c>
-      <c r="X7">
-        <v>1</v>
+      <c r="X7" t="s">
+        <v>124</v>
       </c>
       <c r="Y7">
         <v>1</v>
@@ -4878,16 +4887,16 @@
       <c r="I8" t="s">
         <v>103</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="3">
         <v>36892</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="3">
         <v>36892</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="4">
         <v>4.9305555555555554E-2</v>
       </c>
       <c r="N8" t="s">
@@ -4920,8 +4929,8 @@
       <c r="W8">
         <v>1</v>
       </c>
-      <c r="X8">
-        <v>1</v>
+      <c r="X8" t="s">
+        <v>124</v>
       </c>
       <c r="Y8">
         <v>1</v>

</xml_diff>

<commit_message>
E4412_CIDC_9_27_revised - Samples tab completed
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAF781D-DA50-A148-AC16-3F5922CB4DA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972E1F95-8650-E145-93F5-9B6CEE11448E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10940" yWindow="460" windowWidth="25660" windowHeight="15820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10940" yWindow="460" windowWidth="25660" windowHeight="15820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -395,12 +395,25 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{F468AA2D-D374-EE41-A8F6-0AC656D56CE7}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Categorical description of timepoint at which the sample was taken.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{4ECC6B70-B686-3C44-B6EF-B58A54D5B300}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -408,7 +421,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{AA3B25A5-8AF4-0E45-B26A-711632866120}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Trial Participant Identifier. Example: PT123.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{185357F3-A381-C046-8E12-5049FFF2E389}">
       <text>
         <r>
           <rPr>
@@ -421,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{71B7A005-1E85-D948-8D3F-5276D6F82912}">
       <text>
         <r>
           <rPr>
@@ -434,7 +460,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{BDE109C2-1DEA-AE48-894C-1C290A5B2DDE}">
       <text>
         <r>
           <rPr>
@@ -447,51 +473,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{6BEEFACA-8A20-5146-9D7F-D6EE3DAEACD0}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Categorical description of timepoint at which the sample was taken.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The type of material submitted - tumor/normal/etc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Records if a sample processing (blood or tissue) is not compliant with protocol.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -499,7 +486,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{BF7E2992-6D3A-CB4C-A8D0-04536B2E0C2D}">
       <text>
         <r>
           <rPr>
@@ -512,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{492D85D1-8F8A-8A44-8A6C-5F65837FBB7D}">
       <text>
         <r>
           <rPr>
@@ -525,7 +512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{7C51CD31-5746-BA40-821E-B64AF82E0B41}">
       <text>
         <r>
           <rPr>
@@ -538,12 +525,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{DA76A69C-3550-C748-9063-5D9F1E3BC5AE}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -551,12 +538,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{9356160D-4EC7-1746-AB11-7BB845424000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -564,12 +551,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{65E03067-BBFB-1243-91D9-8E4E0F6FFA04}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -577,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
       <text>
         <r>
           <rPr>
@@ -590,7 +577,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
       <text>
         <r>
           <rPr>
@@ -603,7 +590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
       <text>
         <r>
           <rPr>
@@ -616,7 +603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
       <text>
         <r>
           <rPr>
@@ -629,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
       <text>
         <r>
           <rPr>
@@ -642,12 +629,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -655,7 +642,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{D607F072-8A92-F34D-BF3B-4AAC9B07B854}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indication if sample replacement is/was requested.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{6FEC2048-DFE7-1848-9230-04DC000F42BC}">
       <text>
         <r>
           <rPr>
@@ -668,7 +668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{344EA4A5-77AE-4B49-B67A-181BBD2428FC}">
       <text>
         <r>
           <rPr>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="118">
   <si>
     <t>#t</t>
   </si>
@@ -799,12 +799,6 @@
     <t>PROCESSED SAMPLE ID</t>
   </si>
   <si>
-    <t>GENOMIC SOURCE</t>
-  </si>
-  <si>
-    <t>SAMPLE PROCESSING COMPLIANCE</t>
-  </si>
-  <si>
     <t>SAMPLE LOCATION</t>
   </si>
   <si>
@@ -817,15 +811,6 @@
     <t>TYPE OF PRIMARY CONTAINER</t>
   </si>
   <si>
-    <t>QUANTITY</t>
-  </si>
-  <si>
-    <t>SAMPLE VOLUME</t>
-  </si>
-  <si>
-    <t>SAMPLE VOLUME UNITS</t>
-  </si>
-  <si>
     <t>PBMC VIABILITY</t>
   </si>
   <si>
@@ -931,12 +916,6 @@
     <t>Level_1_starting</t>
   </si>
   <si>
-    <t>Tumor</t>
-  </si>
-  <si>
-    <t>Noncompliant_tissue_fixation_over_36_hrs</t>
-  </si>
-  <si>
     <t>Blood</t>
   </si>
   <si>
@@ -1025,6 +1004,42 @@
   </si>
   <si>
     <t>TEST123_pbmc</t>
+  </si>
+  <si>
+    <t>Entry (#)</t>
+  </si>
+  <si>
+    <t>processed sample type</t>
+  </si>
+  <si>
+    <t>Processed sample volume units</t>
+  </si>
+  <si>
+    <t>Plasma</t>
+  </si>
+  <si>
+    <t>Processed sample volume</t>
+  </si>
+  <si>
+    <t>processed sample concentration</t>
+  </si>
+  <si>
+    <t>processed sample concentration units</t>
+  </si>
+  <si>
+    <t>quality of sample</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Material Storage Condition</t>
+  </si>
+  <si>
+    <t>IDs</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1101,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1142,11 +1157,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -1157,6 +1192,9 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1165,6 +1203,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,7 +1553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1520,13 +1567,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1536,7 +1583,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1547,10 +1594,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1578,7 +1625,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1589,10 +1636,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1620,7 +1667,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1634,7 +1681,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1648,7 +1695,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1662,7 +1709,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1704,7 +1751,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1718,7 +1765,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1732,7 +1779,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -2790,22 +2837,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2847,34 +2894,34 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" t="s">
         <v>58</v>
       </c>
-      <c r="D3" t="s">
+      <c r="I3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" t="s">
+      <c r="J3" t="s">
         <v>60</v>
       </c>
-      <c r="F3" t="s">
+      <c r="K3" t="s">
         <v>61</v>
-      </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -2882,34 +2929,34 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" t="s">
         <v>59</v>
       </c>
-      <c r="E4" t="s">
+      <c r="J4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>61</v>
-      </c>
-      <c r="G4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -2917,34 +2964,34 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" t="s">
         <v>59</v>
       </c>
-      <c r="E5" t="s">
+      <c r="J5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" t="s">
+      <c r="K5" t="s">
         <v>61</v>
-      </c>
-      <c r="G5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -2952,34 +2999,34 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
         <v>58</v>
       </c>
-      <c r="D6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" t="s">
-        <v>63</v>
-      </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2987,34 +3034,34 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
         <v>58</v>
       </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" t="s">
-        <v>63</v>
-      </c>
       <c r="I7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="K7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -3022,34 +3069,34 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="K8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -4061,601 +4108,655 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:X202"/>
+  <dimension ref="A1:AA202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="96" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="96" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4" t="s">
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="W2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="W2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
         <v>52</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="I3">
+        <v>123</v>
+      </c>
+      <c r="J3" t="s">
         <v>76</v>
       </c>
-      <c r="C3" t="s">
+      <c r="K3" t="s">
         <v>77</v>
       </c>
-      <c r="D3" t="s">
+      <c r="L3" t="s">
         <v>78</v>
       </c>
-      <c r="E3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J3">
-        <v>123</v>
-      </c>
-      <c r="K3" t="s">
-        <v>83</v>
-      </c>
-      <c r="L3" t="s">
-        <v>84</v>
-      </c>
       <c r="M3" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
+      <c r="O3" t="s">
+        <v>95</v>
+      </c>
+      <c r="P3">
+        <v>0.2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>79</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
-      <c r="S3" t="s">
-        <v>100</v>
-      </c>
-      <c r="T3">
+      <c r="S3">
         <v>1</v>
       </c>
+      <c r="T3" t="s">
+        <v>93</v>
+      </c>
       <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
         <v>0</v>
       </c>
-      <c r="V3" t="s">
-        <v>87</v>
-      </c>
       <c r="W3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="X3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>90</v>
+      <c r="B4">
+        <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4">
+        <v>123</v>
+      </c>
+      <c r="J4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" t="s">
         <v>77</v>
       </c>
-      <c r="D4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="L4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" t="s">
+        <v>109</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
+        <v>95</v>
+      </c>
+      <c r="P4">
+        <v>0.3</v>
+      </c>
+      <c r="Q4" t="s">
         <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" t="s">
-        <v>82</v>
-      </c>
-      <c r="J4">
-        <v>123</v>
-      </c>
-      <c r="K4" t="s">
-        <v>83</v>
-      </c>
-      <c r="L4" t="s">
-        <v>84</v>
-      </c>
-      <c r="M4" t="s">
-        <v>85</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
       </c>
       <c r="R4">
         <v>1</v>
       </c>
-      <c r="S4" t="s">
-        <v>101</v>
-      </c>
-      <c r="T4">
+      <c r="S4">
         <v>1</v>
       </c>
+      <c r="T4" t="s">
+        <v>94</v>
+      </c>
       <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
         <v>0</v>
       </c>
-      <c r="V4" t="s">
-        <v>87</v>
-      </c>
       <c r="W4" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="X4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>92</v>
+      <c r="B5">
+        <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5">
+        <v>123</v>
+      </c>
+      <c r="J5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" t="s">
         <v>77</v>
       </c>
-      <c r="D5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="L5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5" t="s">
+        <v>95</v>
+      </c>
+      <c r="P5">
+        <v>0.2</v>
+      </c>
+      <c r="Q5" t="s">
         <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" t="s">
-        <v>82</v>
-      </c>
-      <c r="J5">
-        <v>123</v>
-      </c>
-      <c r="K5" t="s">
-        <v>83</v>
-      </c>
-      <c r="L5" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
       </c>
       <c r="R5">
         <v>1</v>
       </c>
-      <c r="S5" t="s">
-        <v>86</v>
-      </c>
-      <c r="T5">
+      <c r="S5">
         <v>1</v>
       </c>
+      <c r="T5" t="s">
+        <v>79</v>
+      </c>
       <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
         <v>0</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
+        <v>95</v>
+      </c>
+      <c r="X5" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
         <v>87</v>
       </c>
-      <c r="W5" t="s">
+      <c r="F6" t="s">
         <v>88</v>
       </c>
-      <c r="X5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6">
+        <v>123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>76</v>
+      </c>
+      <c r="K6" t="s">
         <v>77</v>
       </c>
-      <c r="D6" t="s">
+      <c r="L6" t="s">
+        <v>78</v>
+      </c>
+      <c r="M6" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6" t="s">
         <v>95</v>
       </c>
-      <c r="E6" t="s">
+      <c r="P6">
+        <v>0.2</v>
+      </c>
+      <c r="Q6" t="s">
         <v>79</v>
-      </c>
-      <c r="F6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G6" t="s">
-        <v>80</v>
-      </c>
-      <c r="H6" t="s">
-        <v>81</v>
-      </c>
-      <c r="I6" t="s">
-        <v>82</v>
-      </c>
-      <c r="J6">
-        <v>123</v>
-      </c>
-      <c r="K6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L6" t="s">
-        <v>84</v>
-      </c>
-      <c r="M6" t="s">
-        <v>85</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
       </c>
       <c r="R6">
         <v>1</v>
       </c>
-      <c r="S6" t="s">
-        <v>102</v>
-      </c>
-      <c r="T6">
+      <c r="S6">
         <v>1</v>
       </c>
+      <c r="T6" t="s">
+        <v>95</v>
+      </c>
       <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
         <v>0</v>
       </c>
-      <c r="V6" t="s">
-        <v>87</v>
-      </c>
       <c r="W6" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X6" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7">
+        <v>123</v>
+      </c>
+      <c r="J7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s">
         <v>77</v>
       </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="L7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" t="s">
+        <v>109</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7" t="s">
+        <v>95</v>
+      </c>
+      <c r="P7">
+        <v>0.2</v>
+      </c>
+      <c r="Q7" t="s">
         <v>79</v>
-      </c>
-      <c r="F7" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" t="s">
-        <v>81</v>
-      </c>
-      <c r="I7" t="s">
-        <v>82</v>
-      </c>
-      <c r="J7">
-        <v>123</v>
-      </c>
-      <c r="K7" t="s">
-        <v>83</v>
-      </c>
-      <c r="L7" t="s">
-        <v>84</v>
-      </c>
-      <c r="M7" t="s">
-        <v>85</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q7">
-        <v>1</v>
       </c>
       <c r="R7">
         <v>1</v>
       </c>
-      <c r="S7" t="s">
-        <v>102</v>
-      </c>
-      <c r="T7">
+      <c r="S7">
         <v>1</v>
       </c>
+      <c r="T7" t="s">
+        <v>95</v>
+      </c>
       <c r="U7">
+        <v>1</v>
+      </c>
+      <c r="V7">
         <v>0</v>
       </c>
-      <c r="V7" t="s">
-        <v>87</v>
-      </c>
       <c r="W7" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" t="s">
-        <v>98</v>
+      <c r="B8">
+        <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8">
+        <v>123</v>
+      </c>
+      <c r="J8" t="s">
+        <v>76</v>
+      </c>
+      <c r="K8" t="s">
         <v>77</v>
       </c>
-      <c r="D8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="L8" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" t="s">
+        <v>109</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+      <c r="O8" t="s">
+        <v>95</v>
+      </c>
+      <c r="P8">
+        <v>0.3</v>
+      </c>
+      <c r="Q8" t="s">
         <v>79</v>
-      </c>
-      <c r="F8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" t="s">
-        <v>80</v>
-      </c>
-      <c r="H8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I8" t="s">
-        <v>82</v>
-      </c>
-      <c r="J8">
-        <v>123</v>
-      </c>
-      <c r="K8" t="s">
-        <v>83</v>
-      </c>
-      <c r="L8" t="s">
-        <v>84</v>
-      </c>
-      <c r="M8" t="s">
-        <v>85</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
       </c>
       <c r="R8">
         <v>1</v>
       </c>
-      <c r="S8" t="s">
-        <v>102</v>
-      </c>
-      <c r="T8">
+      <c r="S8">
         <v>1</v>
       </c>
+      <c r="T8" t="s">
+        <v>95</v>
+      </c>
       <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
         <v>0</v>
       </c>
-      <c r="V8" t="s">
-        <v>87</v>
-      </c>
       <c r="W8" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="X8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -5591,33 +5692,34 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="Q1:X1"/>
+  <mergeCells count="3">
+    <mergeCell ref="R1:AA1"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:Q1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H202" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H9 H17:H202" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I202" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Compliant_processing,Noncompliant_tissue_fixation_24_to_36_hrs,Noncompliant_tissue_fixation_over_36_hrs,Noncompliant_blood_processing_ 24_to_48_hrs,Noncompliant_blood_processing_over_48_hrs,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K202" xr:uid="{00000000-0002-0000-0200-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K202 J3:J8" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Stool,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L202" xr:uid="{00000000-0002-0000-0200-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9:L202 K3:K8" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"Blood Draw,Excision,Core Biopsy,Punch Biopsy,Endoscopic Biopsy,Bone Marrow Core Biopsy,Bone Marrow Aspirate,Lumbar Puncture,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M202" xr:uid="{00000000-0002-0000-0200-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M202 L3:L8" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>"Sodium heparin,Blood specimen container with EDTA,Potassium EDTA,Streck Blood Collection Tube,Stool collection container with DNA stabilizer,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P202" xr:uid="{00000000-0002-0000-0200-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P9:P202 Q3:Q8" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"Microliter,Milliliter,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V9:V202 W3:W8" xr:uid="{00000000-0002-0000-0200-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V19:V202 W9 Z3:Z8" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W9:W202 X3:X8" xr:uid="{00000000-0002-0000-0200-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W19:W202 X9 AA3:AA8" xr:uid="{00000000-0002-0000-0200-00000B000000}">
       <formula1>"Sample Returned,Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update manifests - courier & receiving party
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429F289C-7838-CE43-8C4F-7FE8B0DBE013}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDE1471-B263-164E-9178-3FF9995B8F1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="35500" windowHeight="13820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -963,9 +963,6 @@
     <t>Olink</t>
   </si>
   <si>
-    <t>MDA_CIMAC</t>
-  </si>
-  <si>
     <t>USPS</t>
   </si>
   <si>
@@ -1165,6 +1162,9 @@
   </si>
   <si>
     <t>Box number</t>
+  </si>
+  <si>
+    <t>Adaptive Biotechnologies</t>
   </si>
 </sst>
 </file>
@@ -1670,8 +1670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1756,7 +1756,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>131</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1770,7 +1770,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1784,7 +1784,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1798,7 +1798,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1812,7 +1812,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1854,7 +1854,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1868,7 +1868,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1882,7 +1882,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -3016,43 +3016,43 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" t="s">
-        <v>127</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>73</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>74</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>75</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>76</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>77</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>78</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>79</v>
-      </c>
-      <c r="O3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -3063,43 +3063,43 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4" t="s">
         <v>73</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>74</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>75</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>76</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>77</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>78</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>79</v>
-      </c>
-      <c r="O4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -3110,43 +3110,43 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" t="s">
         <v>73</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>74</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>75</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>76</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>77</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>78</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>79</v>
-      </c>
-      <c r="O5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -3157,43 +3157,43 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>74</v>
+      </c>
+      <c r="K6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" t="s">
         <v>83</v>
       </c>
-      <c r="E6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J6" t="s">
-        <v>75</v>
-      </c>
-      <c r="K6" t="s">
-        <v>76</v>
-      </c>
-      <c r="L6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>84</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>85</v>
-      </c>
-      <c r="O6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -3204,43 +3204,43 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" t="s">
         <v>73</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>74</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>75</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>76</v>
       </c>
-      <c r="L7" t="s">
-        <v>77</v>
-      </c>
       <c r="M7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" t="s">
         <v>84</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>85</v>
-      </c>
-      <c r="O7" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -3251,43 +3251,43 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" t="s">
         <v>73</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>74</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>75</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>76</v>
       </c>
-      <c r="L8" t="s">
-        <v>77</v>
-      </c>
       <c r="M8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8" t="s">
         <v>84</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>85</v>
-      </c>
-      <c r="O8" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
@@ -4305,7 +4305,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I33"/>
     </sheetView>
   </sheetViews>
@@ -4377,7 +4377,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>42</v>
@@ -4445,22 +4445,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" t="s">
         <v>107</v>
       </c>
-      <c r="G3" t="s">
-        <v>108</v>
-      </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -4469,28 +4469,28 @@
         <v>123</v>
       </c>
       <c r="K3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" t="s">
         <v>109</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>110</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>111</v>
-      </c>
-      <c r="N3" t="s">
-        <v>112</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q3">
         <v>0.2</v>
       </c>
       <c r="R3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -4499,7 +4499,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V3">
         <v>1</v>
@@ -4508,19 +4508,19 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y3" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z3" t="s">
         <v>116</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>117</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>118</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -4531,22 +4531,22 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
         <v>128</v>
       </c>
-      <c r="D4" t="s">
-        <v>129</v>
-      </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -4555,28 +4555,28 @@
         <v>123</v>
       </c>
       <c r="K4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" t="s">
         <v>109</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>110</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>111</v>
-      </c>
-      <c r="N4" t="s">
-        <v>112</v>
       </c>
       <c r="O4">
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q4">
         <v>0.3</v>
       </c>
       <c r="R4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -4585,7 +4585,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="V4">
         <v>1</v>
@@ -4594,16 +4594,16 @@
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA4" t="s">
         <v>117</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
@@ -4614,22 +4614,22 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -4638,28 +4638,28 @@
         <v>123</v>
       </c>
       <c r="K5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L5" t="s">
         <v>109</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>110</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>111</v>
-      </c>
-      <c r="N5" t="s">
-        <v>112</v>
       </c>
       <c r="O5">
         <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q5">
         <v>0.2</v>
       </c>
       <c r="R5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -4668,7 +4668,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V5">
         <v>1</v>
@@ -4677,16 +4677,16 @@
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y5" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z5" t="s">
         <v>116</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>117</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -4697,22 +4697,22 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -4721,28 +4721,28 @@
         <v>123</v>
       </c>
       <c r="K6" t="s">
+        <v>108</v>
+      </c>
+      <c r="L6" t="s">
         <v>109</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>110</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>111</v>
-      </c>
-      <c r="N6" t="s">
-        <v>112</v>
       </c>
       <c r="O6">
         <v>4</v>
       </c>
       <c r="P6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q6">
         <v>0.2</v>
       </c>
       <c r="R6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -4751,7 +4751,7 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V6">
         <v>1</v>
@@ -4760,16 +4760,16 @@
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA6" t="s">
         <v>117</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -4780,22 +4780,22 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -4804,28 +4804,28 @@
         <v>123</v>
       </c>
       <c r="K7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" t="s">
         <v>109</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>110</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>111</v>
-      </c>
-      <c r="N7" t="s">
-        <v>112</v>
       </c>
       <c r="O7">
         <v>5</v>
       </c>
       <c r="P7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q7">
         <v>0.2</v>
       </c>
       <c r="R7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -4834,7 +4834,7 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V7">
         <v>1</v>
@@ -4843,16 +4843,16 @@
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y7" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z7" t="s">
         <v>116</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>117</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
@@ -4863,22 +4863,22 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -4887,28 +4887,28 @@
         <v>123</v>
       </c>
       <c r="K8" t="s">
+        <v>108</v>
+      </c>
+      <c r="L8" t="s">
         <v>109</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>110</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>111</v>
-      </c>
-      <c r="N8" t="s">
-        <v>112</v>
       </c>
       <c r="O8">
         <v>6</v>
       </c>
       <c r="P8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q8">
         <v>0.3</v>
       </c>
       <c r="R8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -4917,7 +4917,7 @@
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="V8">
         <v>1</v>
@@ -4926,16 +4926,16 @@
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA8" t="s">
         <v>117</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add diagnosis verification to pbmc template
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDE1471-B263-164E-9178-3FF9995B8F1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC08C5BB-3E8A-714F-9CC6-1FCE8D90E800}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="4780" windowWidth="27260" windowHeight="11660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -118,12 +118,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -131,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -157,7 +157,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -170,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -196,7 +196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -306,7 +306,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Descritpion of the topography category. e.g LUNG AND BRONCHUS</t>
+          <t>Indicates whether the local pathology review was consistent with the diagnostic pathology report.</t>
         </r>
       </text>
     </comment>
@@ -319,7 +319,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ICD-0-3 topography site code from which a specimen was isolated. e.g. C34.1</t>
+          <t>Descritpion of the topography category. e.g LUNG AND BRONCHUS</t>
         </r>
       </text>
     </comment>
@@ -332,7 +332,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ICD-0-3 site code description. e.g. Upper lobe, lung</t>
+          <t>ICD-0-3 topography site code from which a specimen was isolated. e.g. C34.1</t>
         </r>
       </text>
     </comment>
@@ -345,7 +345,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ICD-0-3 code for histology and behavior. e.g. 9665/3</t>
+          <t>ICD-0-3 site code description. e.g. Upper lobe, lung</t>
         </r>
       </text>
     </comment>
@@ -358,7 +358,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ICD-0-3 histology and behavior code description. e.g. Hodgkin lymphoma, nod. scler., grade 1</t>
+          <t>ICD-0-3 code for histology and behavior. e.g. 9665/3</t>
         </r>
       </text>
     </comment>
@@ -371,11 +371,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>ICD-0-3 histology and behavior code description. e.g. Hodgkin lymphoma, nod. scler., grade 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Identifies the gender of the participant.</t>
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -389,7 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000E000000}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -418,7 +431,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -431,7 +444,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -504,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{8B674781-FD4D-AB47-BABF-74F3B73AFDF5}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -517,12 +530,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -530,12 +543,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -543,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -556,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -569,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -582,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -595,7 +608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -608,7 +621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
       <text>
         <r>
           <rPr>
@@ -621,7 +634,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
       <text>
         <r>
           <rPr>
@@ -634,12 +647,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -647,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
       <text>
         <r>
           <rPr>
@@ -660,7 +673,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
       <text>
         <r>
           <rPr>
@@ -673,7 +686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
       <text>
         <r>
           <rPr>
@@ -686,7 +699,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
       <text>
         <r>
           <rPr>
@@ -699,7 +712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
       <text>
         <r>
           <rPr>
@@ -712,7 +725,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
       <text>
         <r>
           <rPr>
@@ -725,7 +738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
       <text>
         <r>
           <rPr>
@@ -738,7 +751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -751,7 +764,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
+    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -769,7 +782,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="134">
   <si>
     <t>#t</t>
   </si>
@@ -855,6 +868,9 @@
     <t>Collection event name</t>
   </si>
   <si>
+    <t>Diagnosis verification</t>
+  </si>
+  <si>
     <t>Site description</t>
   </si>
   <si>
@@ -897,6 +913,9 @@
     <t>Processed sample id</t>
   </si>
   <si>
+    <t>Box number</t>
+  </si>
+  <si>
     <t>Sample location</t>
   </si>
   <si>
@@ -963,6 +982,9 @@
     <t>Olink</t>
   </si>
   <si>
+    <t>Adaptive Biotechnologies</t>
+  </si>
+  <si>
     <t>USPS</t>
   </si>
   <si>
@@ -984,9 +1006,87 @@
     <t>ship to</t>
   </si>
   <si>
+    <t>TEST-PAR1-01</t>
+  </si>
+  <si>
     <t>CM-TEST-PAR1-01</t>
   </si>
   <si>
+    <t>Surgical pathology report 1</t>
+  </si>
+  <si>
+    <t>clinical report 1</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>TEST-PAR1-02</t>
+  </si>
+  <si>
+    <t>CM-TEST-PAR1-02</t>
+  </si>
+  <si>
+    <t>Surgical pathology report 2</t>
+  </si>
+  <si>
+    <t>clinical report 2</t>
+  </si>
+  <si>
+    <t>TEST-PAR1-03</t>
+  </si>
+  <si>
+    <t>CM-TEST-PAR1-03</t>
+  </si>
+  <si>
+    <t>Surgical pathology report 3</t>
+  </si>
+  <si>
+    <t>clinical report 3</t>
+  </si>
+  <si>
+    <t>Pre_Day_1_Cycle_2</t>
+  </si>
+  <si>
+    <t>TEST-PAR2-01</t>
+  </si>
+  <si>
+    <t>CM-TEST-PAR2-01</t>
+  </si>
+  <si>
+    <t>Surgical pathology report 4</t>
+  </si>
+  <si>
+    <t>clinical report 4</t>
+  </si>
+  <si>
+    <t>TEST-PAR2-02</t>
+  </si>
+  <si>
+    <t>CM-TEST-PAR2-02</t>
+  </si>
+  <si>
+    <t>Surgical pathology report 5</t>
+  </si>
+  <si>
+    <t>clinical report 5</t>
+  </si>
+  <si>
+    <t>TEST-PAR2-03</t>
+  </si>
+  <si>
+    <t>CM-TEST-PAR2-03</t>
+  </si>
+  <si>
+    <t>Surgical pathology report 6</t>
+  </si>
+  <si>
+    <t>clinical report 6</t>
+  </si>
+  <si>
+    <t>Local pathology review was not consistent</t>
+  </si>
+  <si>
     <t>ANAL CANAL &amp; ANUS</t>
   </si>
   <si>
@@ -1011,15 +1111,6 @@
     <t>Hispanic or Latino</t>
   </si>
   <si>
-    <t>CM-TEST-PAR1-02</t>
-  </si>
-  <si>
-    <t>CM-TEST-PAR1-03</t>
-  </si>
-  <si>
-    <t>CM-TEST-PAR2-01</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -1029,64 +1120,7 @@
     <t>Unknown</t>
   </si>
   <si>
-    <t>CM-TEST-PAR2-02</t>
-  </si>
-  <si>
-    <t>CM-TEST-PAR2-03</t>
-  </si>
-  <si>
-    <t>clinical report 1</t>
-  </si>
-  <si>
-    <t>clinical report 2</t>
-  </si>
-  <si>
-    <t>clinical report 3</t>
-  </si>
-  <si>
-    <t>clinical report 4</t>
-  </si>
-  <si>
-    <t>clinical report 5</t>
-  </si>
-  <si>
-    <t>clinical report 6</t>
-  </si>
-  <si>
-    <t>Surgical pathology report 1</t>
-  </si>
-  <si>
-    <t>Surgical pathology report 2</t>
-  </si>
-  <si>
-    <t>Surgical pathology report 3</t>
-  </si>
-  <si>
-    <t>Surgical pathology report 4</t>
-  </si>
-  <si>
-    <t>Surgical pathology report 5</t>
-  </si>
-  <si>
-    <t>Surgical pathology report 6</t>
-  </si>
-  <si>
-    <t>TEST-PAR1-01</t>
-  </si>
-  <si>
-    <t>TEST-PAR1-02</t>
-  </si>
-  <si>
-    <t>TEST-PAR1-03</t>
-  </si>
-  <si>
-    <t>TEST-PAR2-01</t>
-  </si>
-  <si>
-    <t>TEST-PAR2-02</t>
-  </si>
-  <si>
-    <t>TEST-PAR2-03</t>
+    <t>Arm_Z</t>
   </si>
   <si>
     <t>TRIALGROUP 1</t>
@@ -1140,6 +1174,9 @@
     <t>TRIALGROUP 3</t>
   </si>
   <si>
+    <t>Arm_A</t>
+  </si>
+  <si>
     <t>TRIALGROUP 4</t>
   </si>
   <si>
@@ -1147,31 +1184,13 @@
   </si>
   <si>
     <t>TRIALGROUP 6</t>
-  </si>
-  <si>
-    <t>Baseline</t>
-  </si>
-  <si>
-    <t>Pre_Day_1_Cycle_2</t>
-  </si>
-  <si>
-    <t>Arm_Z</t>
-  </si>
-  <si>
-    <t>Arm_A</t>
-  </si>
-  <si>
-    <t>Box number</t>
-  </si>
-  <si>
-    <t>Adaptive Biotechnologies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1190,18 +1209,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1232,7 +1239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1266,48 +1273,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -1315,20 +1285,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1670,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1684,13 +1645,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1700,7 +1661,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1714,7 +1675,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1742,7 +1703,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1756,7 +1717,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1770,7 +1731,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1784,7 +1745,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1798,7 +1759,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1812,7 +1773,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1825,7 +1786,7 @@
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>37174</v>
       </c>
       <c r="D11" s="1"/>
@@ -1839,7 +1800,7 @@
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>37539</v>
       </c>
       <c r="D12" s="1"/>
@@ -1854,7 +1815,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1868,7 +1829,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1882,7 +1843,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2898,26 +2859,26 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{46309C88-ABE9-3B44-9E22-6D6E54AE7185}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{DB185BF7-7E43-374E-A304-2D40824042A9}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{DA92773C-464B-2946-BCC9-BFE9602054EB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E4C2758A-AEC5-3D43-ABC2-1711081C1AA0}">
       <formula1>"Olink,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{4ECECD59-B204-C141-B575-7C5FAF5F4979}">
-      <formula1>"MDA_CIMAC,MSSM_CIMAC,STAN_CIMAC,DFCI_CIMAC,Broad_CIMAC,FNLCR_MoCha,Nationwide Children's Hospital,Adaptive Biotechnologies,Not Reported,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{F7D20FE0-A831-E948-B268-CF0ED8C27BA2}">
+      <formula1>"Frozen_Dry_Ice,Frozen_Shipper,Ice_Pack,Ambient,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{76D604CF-3E39-E14E-94B7-7F106E388C5E}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C11:C12" xr:uid="{A6B1640B-CCF1-0045-883C-D7A34CF3BDE2}">
+      <formula1>AND(ISNUMBER(C11),LEFT(CELL("format",C11),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{74FEB6F1-8D37-D141-A5B1-AD65D374CC5C}">
+      <formula1>"Specimen shipment received in good condition,Specimen shipment received in poor condition,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{DEE39C81-7A2A-FE45-BD95-2D2E3FD41CB0}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{FB63058B-7B2C-094F-8E15-19E8F00D297D}">
-      <formula1>"Frozen_Dry_Ice,Frozen_Shipper,Ice_Pack,Ambient,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C11:C12" xr:uid="{C57D9D1F-8312-1841-8B4C-8FB84F3DCD08}">
-      <formula1>AND(ISNUMBER(C11),LEFT(CELL("format",C11),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{837EA010-81A2-5141-AAD8-27DD165838BA}">
-      <formula1>"Specimen shipment received in good condition,Specimen shipment received in poor condition,Not Reported,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{6329D08D-3156-B845-A305-1788BBA09B7C}">
+      <formula1>"MDA_CIMAC,MSSM_CIMAC,STAN_CIMAC,DFCI_CIMAC,Broad_CIMAC,FNLCR_MoCha,Nationwide Children's Hospital,Adaptive Biotechnologies,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2927,10 +2888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O202"/>
+  <dimension ref="A1:P202"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2939,29 +2900,30 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -3007,8 +2969,11 @@
       <c r="O2" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -3016,46 +2981,49 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H3" t="s">
         <v>100</v>
       </c>
-      <c r="D3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H3" t="s">
-        <v>72</v>
-      </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="J3" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="L3" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="M3" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="N3" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="O3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="P3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -3063,46 +3031,49 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
         <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="K4" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="L4" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="M4" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="N4" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="O4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="P4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -3110,46 +3081,49 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J5" t="s">
         <v>102</v>
       </c>
-      <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H5" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J5" t="s">
-        <v>74</v>
-      </c>
       <c r="K5" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="L5" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="M5" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="N5" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="O5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="P5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3157,46 +3131,49 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F6" t="s">
         <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>100</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="J6" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="K6" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="M6" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="N6" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="O6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="P6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3204,46 +3181,49 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L7" t="s">
         <v>104</v>
       </c>
-      <c r="D7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J7" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" t="s">
-        <v>75</v>
-      </c>
-      <c r="L7" t="s">
-        <v>76</v>
-      </c>
       <c r="M7" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="N7" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="O7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="P7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3251,81 +3231,84 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" t="s">
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
+        <v>101</v>
+      </c>
+      <c r="J8" t="s">
+        <v>102</v>
+      </c>
+      <c r="K8" t="s">
+        <v>103</v>
+      </c>
+      <c r="L8" t="s">
+        <v>104</v>
+      </c>
+      <c r="M8" t="s">
         <v>105</v>
       </c>
-      <c r="D8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" t="s">
-        <v>126</v>
-      </c>
-      <c r="H8" t="s">
-        <v>72</v>
-      </c>
-      <c r="I8" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" t="s">
-        <v>74</v>
-      </c>
-      <c r="K8" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" t="s">
-        <v>76</v>
-      </c>
-      <c r="M8" t="s">
-        <v>83</v>
-      </c>
       <c r="N8" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="O8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="P8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -4262,38 +4245,40 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="N1:P1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="9">
+  <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G202" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Baseline,Pre_Day_1_Cycle_2,Restaging,Off_study"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M202" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H9:H202" xr:uid="{00000000-0002-0000-0100-000001000000}">
+      <formula1>"Local pathology review was not consistent,Local pathology review was consistent with site of tissue procurement diagnostic pathology report,Not Available,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N202" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Male,Female,Not Specified,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N202" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O202" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"American Indian/Alaska Native,Asian,Black/African American,Native Hawaiian/Pacific Islander,White,Not Reported,Unknown,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O202" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P202" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"Hispanic or Latino,Not Hispanic or Latino,Not reported,Unknown,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L8" xr:uid="{99AC5D7C-8D2B-B14D-A3D7-5F38F6A3B9DD}">
-      <formula1>"Neoplasm, malignant,Tumor cells, malignant,Malignant tumor, small cell type,Malignant tumor, giant cell type,Malignant tumor, spindle cell type,Malignant tumor, clear cell type"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I8" xr:uid="{6B8DFD7B-6F56-7A49-A6DB-DB437F7C019F}">
+      <formula1>"ACCESSORY SINUS, NOS,ADRENAL GLANDS,ANAL CANAL &amp; ANUS,APPENDIX,BASE OF TONGUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K8" xr:uid="{48F48100-F2BB-0746-A24F-8F4E3AC3185C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J8" xr:uid="{C920DFB7-5488-3545-B4FE-6656B85E2F4C}">
+      <formula1>"C00,C00.0,C00.1,C00.2,C00.3,C00.4,C00.5,C00.6,C00.8,C00.9,C01,C01.9"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K8" xr:uid="{A04E0B19-147A-B141-B293-241DEF03DC47}">
+      <formula1>"LIP,External upper lip,External lower lip,External lip, NOS,Mucosa of upper lip,Mucosa of lower lip,Mucosa of lip, NOS,Commissure of lip,Overlapping lesion of lip,Lip, NOS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L8" xr:uid="{B3474AB2-1551-9B4A-B6E8-74D592D4D099}">
       <formula1>"8000/3,8001/3,8002/3,8003/3,8004/3,8005/3,8010/2,8010/3,8011/3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J8" xr:uid="{E9D9BF4A-70C0-B244-A581-DA1C2CBC7681}">
-      <formula1>"LIP,External upper lip,External lower lip,External lip, NOS,Mucosa of upper lip,Mucosa of lower lip,Mucosa of lip, NOS,Commissure of lip,Overlapping lesion of lip,Lip, NOS"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I8" xr:uid="{D468DB17-630F-184E-A0B7-F14937E13EE7}">
-      <formula1>"C00,C00.0,C00.1,C00.2,C00.3,C00.4,C00.5,C00.6,C00.8,C00.9,C01,C01.9"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H8" xr:uid="{DA2AB8F3-21A7-5E47-A3FC-A11609FAF92B}">
-      <formula1>"ACCESSORY SINUS, NOS,ADRENAL GLANDS,ANAL CANAL &amp; ANUS,APPENDIX,BASE OF TONGUE"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M8" xr:uid="{28726907-7707-AD46-A255-625F237245CA}">
+      <formula1>"Neoplasm, malignant,Tumor cells, malignant,Malignant tumor, small cell type,Malignant tumor, giant cell type,Malignant tumor, spindle cell type,Malignant tumor, clear cell type"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4305,51 +4290,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB202"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -4362,79 +4346,79 @@
         <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
@@ -4445,22 +4429,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -4469,28 +4453,28 @@
         <v>123</v>
       </c>
       <c r="K3" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="L3" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M3" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="N3" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Q3">
         <v>0.2</v>
       </c>
       <c r="R3" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -4499,7 +4483,7 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="V3">
         <v>1</v>
@@ -4508,19 +4492,19 @@
         <v>0</v>
       </c>
       <c r="X3" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Y3" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="Z3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="AA3" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="AB3" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -4531,19 +4515,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="G4" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H4" t="s">
         <v>80</v>
@@ -4555,28 +4539,28 @@
         <v>123</v>
       </c>
       <c r="K4" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="L4" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M4" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="N4" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="O4">
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Q4">
         <v>0.3</v>
       </c>
       <c r="R4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -4585,7 +4569,7 @@
         <v>1</v>
       </c>
       <c r="U4" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="V4">
         <v>1</v>
@@ -4594,16 +4578,16 @@
         <v>0</v>
       </c>
       <c r="X4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Y4" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="Z4" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="AA4" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
@@ -4614,22 +4598,22 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -4638,28 +4622,28 @@
         <v>123</v>
       </c>
       <c r="K5" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="L5" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M5" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="N5" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="O5">
         <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Q5">
         <v>0.2</v>
       </c>
       <c r="R5" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -4668,7 +4652,7 @@
         <v>1</v>
       </c>
       <c r="U5" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="V5">
         <v>1</v>
@@ -4677,16 +4661,16 @@
         <v>0</v>
       </c>
       <c r="X5" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Y5" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="Z5" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="AA5" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -4697,22 +4681,22 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="G6" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H6" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -4721,28 +4705,28 @@
         <v>123</v>
       </c>
       <c r="K6" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="L6" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M6" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="N6" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="O6">
         <v>4</v>
       </c>
       <c r="P6" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Q6">
         <v>0.2</v>
       </c>
       <c r="R6" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="S6">
         <v>1</v>
@@ -4751,7 +4735,7 @@
         <v>1</v>
       </c>
       <c r="U6" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="V6">
         <v>1</v>
@@ -4760,16 +4744,16 @@
         <v>0</v>
       </c>
       <c r="X6" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="Y6" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="Z6" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="AA6" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -4780,22 +4764,22 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -4804,28 +4788,28 @@
         <v>123</v>
       </c>
       <c r="K7" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="L7" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M7" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="N7" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="O7">
         <v>5</v>
       </c>
       <c r="P7" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Q7">
         <v>0.2</v>
       </c>
       <c r="R7" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="S7">
         <v>1</v>
@@ -4834,7 +4818,7 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="V7">
         <v>1</v>
@@ -4843,16 +4827,16 @@
         <v>0</v>
       </c>
       <c r="X7" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="Y7" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="Z7" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="AA7" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
@@ -4863,22 +4847,22 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="G8" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -4887,28 +4871,28 @@
         <v>123</v>
       </c>
       <c r="K8" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="L8" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M8" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="N8" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="O8">
         <v>6</v>
       </c>
       <c r="P8" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Q8">
         <v>0.3</v>
       </c>
       <c r="R8" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="S8">
         <v>1</v>
@@ -4917,7 +4901,7 @@
         <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="V8">
         <v>1</v>
@@ -4926,16 +4910,16 @@
         <v>0</v>
       </c>
       <c r="X8" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="Y8" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="Z8" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="AA8" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -5911,8 +5895,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:R1"/>
     <mergeCell ref="S1:AB1"/>
-    <mergeCell ref="I1:R1"/>
   </mergeCells>
   <dataValidations count="17">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C202" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -5921,50 +5905,50 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D202" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Arm_Z,Arm_A,Arm_B,Arm_C,Arm_Y,Arm_D,Arm_E,Arm_F,Arm_X,Arm_G,Arm_H,Arm_I"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA8 Y1:Y9 Y18:Y202" xr:uid="{00000000-0002-0000-0200-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K202 J3:J8" xr:uid="{00000000-0002-0000-0200-000002000000}">
+      <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Lymph Node,Stool,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9:L202 K3:K8" xr:uid="{00000000-0002-0000-0200-000003000000}">
+      <formula1>"Blood Draw,Excision,Core Biopsy,Punch Biopsy,Endoscopic Biopsy,Bone Marrow Core Biopsy,Bone Marrow Aspirate,Lumbar Puncture,Aspirate,Fine-Needle Aspiration,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M202" xr:uid="{00000000-0002-0000-0200-000004000000}">
+      <formula1>"Sodium heparin,Blood specimen container with EDTA,Potassium EDTA,Streck Blood Collection Tube,Stool collection container with DNA stabilizer,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9:N202 M3:M8" xr:uid="{00000000-0002-0000-0200-000005000000}">
+      <formula1>"Whole Blood,Plasma,PBMC,Buffy Coat,Bone Marrow Mononuclear Cell,Supernatant,Cell Pellet,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P9:P202 O3:O8" xr:uid="{00000000-0002-0000-0200-000006000000}">
+      <formula1>"µL,mL,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R9:R202 Q3:Q8" xr:uid="{00000000-0002-0000-0200-000007000000}">
+      <formula1>"Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U9:U202 T3:T8" xr:uid="{00000000-0002-0000-0200-000008000000}">
+      <formula1>"Yes,No,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X9:X202 W3:W8" xr:uid="{00000000-0002-0000-0200-000009000000}">
+      <formula1>"RT,4oC,(-20)oC,(-80)oC,LN,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y9:Y202 X3:X8" xr:uid="{00000000-0002-0000-0200-00000A000000}">
+      <formula1>"Pass,Fail,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z9:Z202 AA3:AA8 Y3:Y8" xr:uid="{00000000-0002-0000-0200-00000B000000}">
       <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3:AB8 Z1:Z9 Z18:Z202" xr:uid="{00000000-0002-0000-0200-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA9:AA202 AB3:AB8 Z3:Z8" xr:uid="{00000000-0002-0000-0200-00000C000000}">
       <formula1>"Sample Returned,Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R8" xr:uid="{39BAD97D-1A35-014E-87A2-699C0765C83C}">
-      <formula1>"Microliter,Milliliter,Not Reported,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H8" xr:uid="{3C08D381-A4C4-6D48-8E03-7769FB350AF4}">
+      <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L8" xr:uid="{FD0722EF-FB52-8E4F-8173-D8DA2A481B37}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K8" xr:uid="{6AB79200-D410-1641-A7F3-5A1EDAA8B1AF}">
+      <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Stool,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L8" xr:uid="{1B8B03BD-F437-6041-95C4-90E0E3BC923B}">
       <formula1>"Blood Draw,Excision,Core Biopsy,Punch Biopsy,Endoscopic Biopsy,Bone Marrow Core Biopsy,Bone Marrow Aspirate,Lumbar Puncture,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K8" xr:uid="{8C7A8503-9B29-DF4D-971C-7D521B66E478}">
-      <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Stool,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H8" xr:uid="{10E0B7BD-6007-004C-8C3D-F80087679DAC}">
-      <formula1>"Tumor,Normal,Metastasis"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L18:L202 L9 M3:M8" xr:uid="{00000000-0002-0000-0200-000004000000}">
-      <formula1>"Sodium heparin,Blood specimen container with EDTA,Potassium EDTA,Streck Blood Collection Tube,Stool collection container with DNA stabilizer,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J18:J202 J2:J9 I1" xr:uid="{00000000-0002-0000-0200-000002000000}">
-      <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Lymph Node,Stool,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K18:K202 K2:K9" xr:uid="{00000000-0002-0000-0200-000003000000}">
-      <formula1>"Blood Draw,Excision,Core Biopsy,Punch Biopsy,Endoscopic Biopsy,Bone Marrow Core Biopsy,Bone Marrow Aspirate,Lumbar Puncture,Aspirate,Fine-Needle Aspiration,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M18:M202 M2:M9" xr:uid="{00000000-0002-0000-0200-000005000000}">
-      <formula1>"Whole Blood,Plasma,PBMC,Buffy Coat,Bone Marrow Mononuclear Cell,Supernatant,Cell Pellet,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O18:O202 O2:O9" xr:uid="{00000000-0002-0000-0200-000006000000}">
-      <formula1>"µL,mL,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q18:Q202 Q2:Q9" xr:uid="{00000000-0002-0000-0200-000007000000}">
-      <formula1>"Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T18:T202 T1:T9" xr:uid="{00000000-0002-0000-0200-000008000000}">
-      <formula1>"Yes,No,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W18:W202 W1:W9" xr:uid="{00000000-0002-0000-0200-000009000000}">
-      <formula1>"RT,4oC,(-20)oC,(-80)oC,LN,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X18:X202 X1:X9" xr:uid="{00000000-0002-0000-0200-00000A000000}">
-      <formula1>"Pass,Fail,Not Reported,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R8" xr:uid="{3CDF86FF-777E-DC4B-933A-076D4D4AE862}">
+      <formula1>"Microliter,Milliliter,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update enums for sample_replacement and residual_sample
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC08C5BB-3E8A-714F-9CC6-1FCE8D90E800}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D9CF75-9637-1846-941D-98A0D34E36F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="4780" windowWidth="27260" windowHeight="11660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9520" yWindow="2560" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -973,6 +973,9 @@
     <t>Comments</t>
   </si>
   <si>
+    <t>Replacement Not Requested</t>
+  </si>
+  <si>
     <t>TEST123_pbmc</t>
   </si>
   <si>
@@ -1021,6 +1024,33 @@
     <t>Baseline</t>
   </si>
   <si>
+    <t>Local pathology review was not consistent</t>
+  </si>
+  <si>
+    <t>ANAL CANAL &amp; ANUS</t>
+  </si>
+  <si>
+    <t>C00.1</t>
+  </si>
+  <si>
+    <t>LIP</t>
+  </si>
+  <si>
+    <t>8004/3</t>
+  </si>
+  <si>
+    <t>Neoplasm, malignant</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Hispanic or Latino</t>
+  </si>
+  <si>
     <t>TEST-PAR1-02</t>
   </si>
   <si>
@@ -1060,6 +1090,15 @@
     <t>clinical report 4</t>
   </si>
   <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Native Hawaiian/Pacific Islander</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
     <t>TEST-PAR2-02</t>
   </si>
   <si>
@@ -1084,42 +1123,6 @@
     <t>clinical report 6</t>
   </si>
   <si>
-    <t>Local pathology review was not consistent</t>
-  </si>
-  <si>
-    <t>ANAL CANAL &amp; ANUS</t>
-  </si>
-  <si>
-    <t>C00.1</t>
-  </si>
-  <si>
-    <t>LIP</t>
-  </si>
-  <si>
-    <t>8004/3</t>
-  </si>
-  <si>
-    <t>Neoplasm, malignant</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Asian</t>
-  </si>
-  <si>
-    <t>Hispanic or Latino</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Native Hawaiian/Pacific Islander</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
     <t>Arm_Z</t>
   </si>
   <si>
@@ -1153,44 +1156,41 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>Sample received from CIMAC</t>
+    <t>TRIALGROUP 2</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>TRIALGROUP 3</t>
+  </si>
+  <si>
+    <t>Arm_A</t>
+  </si>
+  <si>
+    <t>TRIALGROUP 4</t>
+  </si>
+  <si>
+    <t>TRIALGROUP 5</t>
+  </si>
+  <si>
+    <t>TRIALGROUP 6</t>
   </si>
   <si>
     <t>Sample Returned</t>
   </si>
   <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 2</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 3</t>
-  </si>
-  <si>
-    <t>Arm_A</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 4</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 5</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1211,6 +1211,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1277,7 +1284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -1291,6 +1298,7 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1631,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
@@ -1661,7 +1669,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1675,7 +1683,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1703,7 +1711,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1717,7 +1725,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1731,7 +1739,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -1745,7 +1753,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1759,7 +1767,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1773,7 +1781,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1815,7 +1823,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1829,7 +1837,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1843,7 +1851,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -2859,25 +2867,25 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{DB185BF7-7E43-374E-A304-2D40824042A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{9567967A-35DE-E345-BC81-026E2BE81B4E}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{E4C2758A-AEC5-3D43-ABC2-1711081C1AA0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{5D98DFC9-054F-A343-9710-19B777E73DF2}">
       <formula1>"Olink,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{F7D20FE0-A831-E948-B268-CF0ED8C27BA2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{D1018D37-89A7-B849-8435-13701DD68BA0}">
       <formula1>"Frozen_Dry_Ice,Frozen_Shipper,Ice_Pack,Ambient,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C11:C12" xr:uid="{A6B1640B-CCF1-0045-883C-D7A34CF3BDE2}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C11:C12" xr:uid="{ED5C4C54-AD8C-F141-904D-5C0B70FEFF0D}">
       <formula1>AND(ISNUMBER(C11),LEFT(CELL("format",C11),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{74FEB6F1-8D37-D141-A5B1-AD65D374CC5C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{4873E571-CF6F-F34F-8B05-01AB11D178D6}">
       <formula1>"Specimen shipment received in good condition,Specimen shipment received in poor condition,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{DEE39C81-7A2A-FE45-BD95-2D2E3FD41CB0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7" xr:uid="{7F828C7C-7C6E-F649-B452-87CD7F96DA61}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{6329D08D-3156-B845-A305-1788BBA09B7C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6" xr:uid="{3D5FE4CE-A8FB-514F-ADA0-C27031AC733F}">
       <formula1>"MDA_CIMAC,MSSM_CIMAC,STAN_CIMAC,DFCI_CIMAC,Broad_CIMAC,FNLCR_MoCha,Nationwide Children's Hospital,Adaptive Biotechnologies,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2890,8 +2898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P202"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:P8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2981,46 +2989,46 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="J3" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="K3" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="L3" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="M3" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="N3" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="O3" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="P3" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -3031,46 +3039,46 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" t="s">
         <v>79</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>80</v>
       </c>
-      <c r="E4" t="s">
+      <c r="I4" t="s">
         <v>81</v>
       </c>
-      <c r="F4" t="s">
+      <c r="J4" t="s">
         <v>82</v>
       </c>
-      <c r="G4" t="s">
-        <v>78</v>
-      </c>
-      <c r="H4" t="s">
-        <v>100</v>
-      </c>
-      <c r="I4" t="s">
-        <v>101</v>
-      </c>
-      <c r="J4" t="s">
-        <v>102</v>
-      </c>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="L4" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="M4" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="N4" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="O4" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="P4" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -3081,46 +3089,46 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" t="s">
         <v>83</v>
       </c>
-      <c r="D5" t="s">
+      <c r="L5" t="s">
         <v>84</v>
       </c>
-      <c r="E5" t="s">
+      <c r="M5" t="s">
         <v>85</v>
       </c>
-      <c r="F5" t="s">
+      <c r="N5" t="s">
         <v>86</v>
       </c>
-      <c r="G5" t="s">
+      <c r="O5" t="s">
         <v>87</v>
       </c>
-      <c r="H5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I5" t="s">
-        <v>101</v>
-      </c>
-      <c r="J5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K5" t="s">
-        <v>103</v>
-      </c>
-      <c r="L5" t="s">
-        <v>104</v>
-      </c>
-      <c r="M5" t="s">
-        <v>105</v>
-      </c>
-      <c r="N5" t="s">
-        <v>106</v>
-      </c>
-      <c r="O5" t="s">
-        <v>107</v>
-      </c>
       <c r="P5" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -3131,46 +3139,46 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="H6" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I6" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" t="s">
         <v>102</v>
       </c>
-      <c r="K6" t="s">
+      <c r="O6" t="s">
         <v>103</v>
       </c>
-      <c r="L6" t="s">
+      <c r="P6" t="s">
         <v>104</v>
-      </c>
-      <c r="M6" t="s">
-        <v>105</v>
-      </c>
-      <c r="N6" t="s">
-        <v>109</v>
-      </c>
-      <c r="O6" t="s">
-        <v>110</v>
-      </c>
-      <c r="P6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -3181,46 +3189,46 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="G7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I7" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="J7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K7" t="s">
+        <v>83</v>
+      </c>
+      <c r="L7" t="s">
+        <v>84</v>
+      </c>
+      <c r="M7" t="s">
+        <v>85</v>
+      </c>
+      <c r="N7" t="s">
         <v>102</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" t="s">
         <v>103</v>
       </c>
-      <c r="L7" t="s">
+      <c r="P7" t="s">
         <v>104</v>
-      </c>
-      <c r="M7" t="s">
-        <v>105</v>
-      </c>
-      <c r="N7" t="s">
-        <v>109</v>
-      </c>
-      <c r="O7" t="s">
-        <v>110</v>
-      </c>
-      <c r="P7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -3231,46 +3239,46 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H8" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I8" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="J8" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" t="s">
+        <v>85</v>
+      </c>
+      <c r="N8" t="s">
         <v>102</v>
       </c>
-      <c r="K8" t="s">
+      <c r="O8" t="s">
         <v>103</v>
       </c>
-      <c r="L8" t="s">
+      <c r="P8" t="s">
         <v>104</v>
-      </c>
-      <c r="M8" t="s">
-        <v>105</v>
-      </c>
-      <c r="N8" t="s">
-        <v>109</v>
-      </c>
-      <c r="O8" t="s">
-        <v>110</v>
-      </c>
-      <c r="P8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -4265,19 +4273,19 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P202" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"Hispanic or Latino,Not Hispanic or Latino,Not reported,Unknown,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I8" xr:uid="{6B8DFD7B-6F56-7A49-A6DB-DB437F7C019F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I8" xr:uid="{7DA72159-1502-B14C-AC02-7897ABFBCB4F}">
       <formula1>"ACCESSORY SINUS, NOS,ADRENAL GLANDS,ANAL CANAL &amp; ANUS,APPENDIX,BASE OF TONGUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J8" xr:uid="{C920DFB7-5488-3545-B4FE-6656B85E2F4C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J8" xr:uid="{230175BF-BB1A-A64F-833E-314118D8AFF7}">
       <formula1>"C00,C00.0,C00.1,C00.2,C00.3,C00.4,C00.5,C00.6,C00.8,C00.9,C01,C01.9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K8" xr:uid="{A04E0B19-147A-B141-B293-241DEF03DC47}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K8" xr:uid="{CF135CDD-DFB6-DD4F-8610-8F4444BDAD85}">
       <formula1>"LIP,External upper lip,External lower lip,External lip, NOS,Mucosa of upper lip,Mucosa of lower lip,Mucosa of lip, NOS,Commissure of lip,Overlapping lesion of lip,Lip, NOS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L8" xr:uid="{B3474AB2-1551-9B4A-B6E8-74D592D4D099}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L8" xr:uid="{03E4CC2A-B175-B341-A33F-74AACE6D12D6}">
       <formula1>"8000/3,8001/3,8002/3,8003/3,8004/3,8005/3,8010/2,8010/3,8011/3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M8" xr:uid="{28726907-7707-AD46-A255-625F237245CA}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M8" xr:uid="{52DDA917-EF74-F649-8F89-81F73DAAE8A7}">
       <formula1>"Neoplasm, malignant,Tumor cells, malignant,Malignant tumor, small cell type,Malignant tumor, giant cell type,Malignant tumor, spindle cell type,Malignant tumor, clear cell type"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4290,8 +4298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:AB8"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4425,501 +4433,501 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="H3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3">
+      <c r="G3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="5">
         <v>1</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="5">
         <v>123</v>
       </c>
-      <c r="K3" t="s">
-        <v>115</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="K3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="M3" t="s">
+      <c r="L3" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="N3" t="s">
+      <c r="M3" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="O3">
+      <c r="N3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O3" s="5">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q3">
+      <c r="P3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q3" s="5">
         <v>0.2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S3" s="5">
+        <v>1</v>
+      </c>
+      <c r="T3" s="5">
+        <v>1</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="V3" s="5">
+        <v>1</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0</v>
+      </c>
+      <c r="X3" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3" t="s">
-        <v>121</v>
-      </c>
-      <c r="V3">
-        <v>1</v>
-      </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>122</v>
+      <c r="Y3" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="Z3" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="AA3" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="AB3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
+        <v>123</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O4" s="5">
+        <v>2</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S4" s="5">
+        <v>1</v>
+      </c>
+      <c r="T4" s="5">
+        <v>1</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="V4" s="5">
+        <v>1</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y4" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="G4" t="s">
-        <v>114</v>
-      </c>
-      <c r="H4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>123</v>
-      </c>
-      <c r="K4" t="s">
-        <v>115</v>
-      </c>
-      <c r="L4" t="s">
-        <v>116</v>
-      </c>
-      <c r="M4" t="s">
-        <v>117</v>
-      </c>
-      <c r="N4" t="s">
-        <v>118</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q4">
-        <v>0.3</v>
-      </c>
-      <c r="R4" t="s">
-        <v>120</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4" t="s">
-        <v>127</v>
-      </c>
-      <c r="V4">
-        <v>1</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>128</v>
-      </c>
       <c r="Z4" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="AA4" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5">
+      <c r="C5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" s="5">
         <v>1</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="5">
         <v>123</v>
       </c>
-      <c r="K5" t="s">
-        <v>115</v>
-      </c>
-      <c r="L5" t="s">
+      <c r="K5" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="M5" t="s">
+      <c r="L5" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="N5" t="s">
+      <c r="M5" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="O5">
+      <c r="N5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O5" s="5">
         <v>3</v>
       </c>
-      <c r="P5" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q5">
+      <c r="P5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q5" s="5">
         <v>0.2</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S5" s="5">
+        <v>1</v>
+      </c>
+      <c r="T5" s="5">
+        <v>1</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="V5" s="5">
+        <v>1</v>
+      </c>
+      <c r="W5" s="5">
+        <v>0</v>
+      </c>
+      <c r="X5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5" t="s">
-        <v>120</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>122</v>
+      <c r="Y5" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="Z5" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="AA5" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" t="s">
-        <v>114</v>
-      </c>
-      <c r="H6" t="s">
-        <v>89</v>
-      </c>
-      <c r="I6">
+      <c r="C6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6" s="5">
         <v>1</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="5">
         <v>123</v>
       </c>
-      <c r="K6" t="s">
-        <v>115</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="K6" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="M6" t="s">
+      <c r="L6" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="N6" t="s">
+      <c r="M6" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="O6">
+      <c r="N6" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O6" s="5">
         <v>4</v>
       </c>
-      <c r="P6" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q6">
+      <c r="P6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q6" s="5">
         <v>0.2</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S6" s="5">
+        <v>1</v>
+      </c>
+      <c r="T6" s="5">
+        <v>1</v>
+      </c>
+      <c r="U6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="S6">
+      <c r="V6" s="5">
         <v>1</v>
       </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6" t="s">
-        <v>119</v>
-      </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6">
+      <c r="W6" s="5">
         <v>0</v>
       </c>
-      <c r="X6" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>128</v>
+      <c r="X6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y6" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="Z6" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="AA6" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5">
+        <v>123</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O7" s="5">
+        <v>5</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S7" s="5">
+        <v>1</v>
+      </c>
+      <c r="T7" s="5">
+        <v>1</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="V7" s="5">
+        <v>1</v>
+      </c>
+      <c r="W7" s="5">
+        <v>0</v>
+      </c>
+      <c r="X7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA7" t="s">
         <v>132</v>
-      </c>
-      <c r="G7" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>123</v>
-      </c>
-      <c r="K7" t="s">
-        <v>115</v>
-      </c>
-      <c r="L7" t="s">
-        <v>116</v>
-      </c>
-      <c r="M7" t="s">
-        <v>117</v>
-      </c>
-      <c r="N7" t="s">
-        <v>118</v>
-      </c>
-      <c r="O7">
-        <v>5</v>
-      </c>
-      <c r="P7" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q7">
-        <v>0.2</v>
-      </c>
-      <c r="R7" t="s">
-        <v>120</v>
-      </c>
-      <c r="S7">
-        <v>1</v>
-      </c>
-      <c r="T7">
-        <v>1</v>
-      </c>
-      <c r="U7" t="s">
-        <v>119</v>
-      </c>
-      <c r="V7">
-        <v>1</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" t="s">
-        <v>133</v>
-      </c>
-      <c r="G8" t="s">
-        <v>114</v>
-      </c>
-      <c r="H8" t="s">
-        <v>97</v>
-      </c>
-      <c r="I8">
+      <c r="C8" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="5">
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="5">
         <v>123</v>
       </c>
-      <c r="K8" t="s">
-        <v>115</v>
-      </c>
-      <c r="L8" t="s">
+      <c r="K8" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="M8" t="s">
+      <c r="L8" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="N8" t="s">
+      <c r="M8" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="O8">
+      <c r="N8" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="O8" s="5">
         <v>6</v>
       </c>
-      <c r="P8" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q8">
+      <c r="P8" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q8" s="5">
         <v>0.3</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R8" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="S8" s="5">
+        <v>1</v>
+      </c>
+      <c r="T8" s="5">
+        <v>1</v>
+      </c>
+      <c r="U8" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="S8">
+      <c r="V8" s="5">
         <v>1</v>
       </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8" t="s">
-        <v>119</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8">
+      <c r="W8" s="5">
         <v>0</v>
       </c>
-      <c r="X8" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>128</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>123</v>
+      <c r="X8" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y8" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z8" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="AA8" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -5898,57 +5906,48 @@
     <mergeCell ref="I1:R1"/>
     <mergeCell ref="S1:AB1"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C202" xr:uid="{00000000-0002-0000-0200-000000000000}">
+  <dataValidations count="14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C202" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Baseline,Pre_Day_1_Cycle_2,Restaging,Off_study"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D202" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D202" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"Arm_Z,Arm_A,Arm_B,Arm_C,Arm_Y,Arm_D,Arm_E,Arm_F,Arm_X,Arm_G,Arm_H,Arm_I"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K202 J3:J8" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K202" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Lymph Node,Stool,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9:L202 K3:K8" xr:uid="{00000000-0002-0000-0200-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9:L202" xr:uid="{00000000-0002-0000-0200-000003000000}">
       <formula1>"Blood Draw,Excision,Core Biopsy,Punch Biopsy,Endoscopic Biopsy,Bone Marrow Core Biopsy,Bone Marrow Aspirate,Lumbar Puncture,Aspirate,Fine-Needle Aspiration,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3:M202" xr:uid="{00000000-0002-0000-0200-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M202" xr:uid="{00000000-0002-0000-0200-000004000000}">
       <formula1>"Sodium heparin,Blood specimen container with EDTA,Potassium EDTA,Streck Blood Collection Tube,Stool collection container with DNA stabilizer,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9:N202 M3:M8" xr:uid="{00000000-0002-0000-0200-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N9:N202" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Whole Blood,Plasma,PBMC,Buffy Coat,Bone Marrow Mononuclear Cell,Supernatant,Cell Pellet,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P9:P202 O3:O8" xr:uid="{00000000-0002-0000-0200-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P9:P202" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"µL,mL,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R9:R202 Q3:Q8" xr:uid="{00000000-0002-0000-0200-000007000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R9:R202" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U9:U202 T3:T8" xr:uid="{00000000-0002-0000-0200-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U9:U202" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>"Yes,No,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X9:X202 W3:W8" xr:uid="{00000000-0002-0000-0200-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X9:X202" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"RT,4oC,(-20)oC,(-80)oC,LN,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y9:Y202 X3:X8" xr:uid="{00000000-0002-0000-0200-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y9:Y202" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"Pass,Fail,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z9:Z202 AA3:AA8 Y3:Y8" xr:uid="{00000000-0002-0000-0200-00000B000000}">
-      <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3:Z202" xr:uid="{00000000-0002-0000-0200-00000B000000}">
+      <formula1>"Replacement Not Requested,Replacement Requested,Replacement Tested,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA9:AA202 AB3:AB8 Z3:Z8" xr:uid="{00000000-0002-0000-0200-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA9:AA202 AB3:AB8" xr:uid="{00000000-0002-0000-0200-00000C000000}">
       <formula1>"Sample Returned,Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H8" xr:uid="{3C08D381-A4C4-6D48-8E03-7769FB350AF4}">
-      <formula1>"Tumor,Normal,Metastasis"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K8" xr:uid="{6AB79200-D410-1641-A7F3-5A1EDAA8B1AF}">
-      <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Stool,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L8" xr:uid="{1B8B03BD-F437-6041-95C4-90E0E3BC923B}">
-      <formula1>"Blood Draw,Excision,Core Biopsy,Punch Biopsy,Endoscopic Biopsy,Bone Marrow Core Biopsy,Bone Marrow Aspirate,Lumbar Puncture,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R8" xr:uid="{3CDF86FF-777E-DC4B-933A-076D4D4AE862}">
-      <formula1>"Microliter,Milliliter,Not Reported,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA8" xr:uid="{88132EE3-597B-2144-9269-DA4470D378A0}">
+      <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prevent overwrites on merge (#209)
* Prevent updates by default in prism

* Update tests

* Revert autoformatting

* Update cidc_schemas/prism.py

Co-Authored-By: Pavel T  <pavel@ds.dfci.harvard.edu>

* Address PR comments and bump version

* Fix failing test
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EAE633-FA5A-1A47-8FA7-0195D14B4743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E4E7CE-C3A1-CF44-94B5-E67CA83B9D31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="2560" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9520" yWindow="2560" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -175,7 +175,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1190,7 +1190,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1218,6 +1218,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1639,7 +1645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -4298,8 +4304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB202"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4440,7 +4446,7 @@
         <v>78</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>74</v>
@@ -4526,7 +4532,7 @@
         <v>96</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>88</v>
@@ -4609,7 +4615,7 @@
         <v>78</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>92</v>
@@ -4692,7 +4698,7 @@
         <v>78</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>97</v>
@@ -4775,7 +4781,7 @@
         <v>96</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>104</v>
@@ -4858,7 +4864,7 @@
         <v>78</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
CIDC-1339 regenerate key manifest template exs
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -896,7 +896,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6724" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6725" uniqueCount="340">
   <si>
     <t xml:space="preserve">#title</t>
   </si>
@@ -1889,6 +1889,9 @@
     <t xml:space="preserve">12</t>
   </si>
   <si>
+    <t xml:space="preserve">ctDNA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Broad_Cibulskis</t>
   </si>
   <si>
@@ -2159,11 +2162,11 @@
   </sheetPr>
   <dimension ref="A1:C2018"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B3:AG8 C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -12394,10 +12397,10 @@
   <dimension ref="A1:P2002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:AG8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -22810,11 +22813,11 @@
   </sheetPr>
   <dimension ref="A1:AG2002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:AG8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -23554,32 +23557,32 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>30</v>
       </c>
@@ -33563,7 +33566,7 @@
       <formula1>'Data Dictionary'!$S$2:$S$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W10:W2002" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="W9:W2002" type="list">
       <formula1>'Data Dictionary'!$T$2:$T$7</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -33659,10 +33662,10 @@
   <dimension ref="B1:E71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:AG8 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -34486,10 +34489,10 @@
   <dimension ref="B1:Y18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:AG8 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -35074,8 +35077,11 @@
       <c r="B13" s="0" t="s">
         <v>329</v>
       </c>
+      <c r="C13" s="0" t="s">
+        <v>330</v>
+      </c>
       <c r="D13" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>121</v>
@@ -35089,10 +35095,10 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O14" s="0" t="s">
         <v>121</v>
@@ -35100,18 +35106,18 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35119,7 +35125,7 @@
         <v>122</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -35127,7 +35133,7 @@
         <v>121</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CIDC-1412 new partic alert and test
</commit_message>
<xml_diff>
--- a/template_examples/pbmc_template.xlsx
+++ b/template_examples/pbmc_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" state="visible" r:id="rId2"/>
@@ -1048,7 +1048,7 @@
     <t xml:space="preserve">TTTP01</t>
   </si>
   <si>
-    <t xml:space="preserve">CTTTP01A1.00</t>
+    <t xml:space="preserve">CTTTP01A4.00</t>
   </si>
   <si>
     <t xml:space="preserve">Surgical pathology report 1</t>
@@ -1087,7 +1087,7 @@
     <t xml:space="preserve">Hispanic or Latino</t>
   </si>
   <si>
-    <t xml:space="preserve">CTTTP01A2.00</t>
+    <t xml:space="preserve">CTTTP01A5.00</t>
   </si>
   <si>
     <t xml:space="preserve">Surgical pathology report 2</t>
@@ -1099,7 +1099,7 @@
     <t xml:space="preserve">Pre_Day_1_Cycle_2</t>
   </si>
   <si>
-    <t xml:space="preserve">CTTTP01A3.00</t>
+    <t xml:space="preserve">CTTTP01A6.00</t>
   </si>
   <si>
     <t xml:space="preserve">Surgical pathology report 3</t>
@@ -1111,7 +1111,7 @@
     <t xml:space="preserve">TTTP02</t>
   </si>
   <si>
-    <t xml:space="preserve">CTTTP02A1.00</t>
+    <t xml:space="preserve">CTTTP02A4.00</t>
   </si>
   <si>
     <t xml:space="preserve">Surgical pathology report 4</t>
@@ -1129,7 +1129,7 @@
     <t xml:space="preserve">Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">CTTTP02A2.00</t>
+    <t xml:space="preserve">CTTTP02A5.00</t>
   </si>
   <si>
     <t xml:space="preserve">Surgical pathology report 5</t>
@@ -1138,7 +1138,7 @@
     <t xml:space="preserve">clinical report 5</t>
   </si>
   <si>
-    <t xml:space="preserve">CTTTP02A3.00</t>
+    <t xml:space="preserve">CTTTP02A6.00</t>
   </si>
   <si>
     <t xml:space="preserve">Surgical pathology report 6</t>
@@ -2163,10 +2163,10 @@
   <dimension ref="A1:C2018"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B3:AG8 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -12396,11 +12396,11 @@
   </sheetPr>
   <dimension ref="A1:P2002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:AG8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -22813,11 +22813,11 @@
   </sheetPr>
   <dimension ref="A1:AG2002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:AG8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S7" activeCellId="0" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -33662,10 +33662,10 @@
   <dimension ref="B1:E71"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:AG8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -34489,10 +34489,10 @@
   <dimension ref="B1:Y18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:AG8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>

</xml_diff>